<commit_message>
Added better vision system
</commit_message>
<xml_diff>
--- a/stories/colddeadwater/data/map.xlsx
+++ b/stories/colddeadwater/data/map.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
-    <workbookView xWindow="10720" yWindow="0" windowWidth="18080" windowHeight="17480" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500"/>
+    <workbookView xWindow="10720" yWindow="0" windowWidth="27680" windowHeight="21080" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="world" sheetId="1" r:id="rId1"/>
-    <sheet name="hq-rooms" sheetId="5" r:id="rId2"/>
-    <sheet name="city-rooms" sheetId="4" r:id="rId3"/>
-    <sheet name="hw-rooms" sheetId="6" r:id="rId4"/>
+    <sheet name="hq-nodes" sheetId="5" r:id="rId2"/>
+    <sheet name="city-nodes" sheetId="4" r:id="rId3"/>
+    <sheet name="hw-nodes" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="470">
   <si>
     <t>.</t>
   </si>
@@ -325,15 +325,15 @@
     <t>.</t>
   </si>
   <si>
+    <t>|</t>
+  </si>
+  <si>
     <t>.</t>
   </si>
   <si>
     <t>.</t>
   </si>
   <si>
-    <t>|</t>
-  </si>
-  <si>
     <t>.</t>
   </si>
   <si>
@@ -379,102 +379,96 @@
     <t>.</t>
   </si>
   <si>
+    <t>%</t>
+  </si>
+  <si>
     <t>.</t>
   </si>
   <si>
+    <t>%</t>
+  </si>
+  <si>
     <t>.</t>
   </si>
   <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>G7</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
     <t>%</t>
   </si>
   <si>
+    <t>G6</t>
+  </si>
+  <si>
     <t>.</t>
   </si>
   <si>
-    <t>%</t>
-  </si>
-  <si>
     <t>.</t>
   </si>
   <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>G3</t>
-  </si>
-  <si>
-    <t>G7</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>G1</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>G2</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>G4</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>G6</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
     <t>G5</t>
   </si>
   <si>
@@ -1424,13 +1418,28 @@
   </si>
   <si>
     <t>Refinery</t>
+  </si>
+  <si>
+    <t>radio m870 m70 mp5 m1911 crowbar crate</t>
+  </si>
+  <si>
+    <t>frag frag</t>
+  </si>
+  <si>
+    <t>tank</t>
+  </si>
+  <si>
+    <t>bertram davide</t>
+  </si>
+  <si>
+    <t>fenton</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1485,6 +1494,10 @@
       <sz val="10"/>
       <name val="Menlo Bold"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Menlo Regular"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1509,7 +1522,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1533,8 +1546,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="163">
+  <cellStyleXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1698,8 +1720,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1764,8 +1796,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="163">
+  <cellStyles count="173">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1847,6 +1900,11 @@
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1928,9 +1986,14 @@
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="7">
     <dxf>
       <font>
         <color theme="9" tint="-0.249977111117893"/>
@@ -2001,66 +2064,6 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.249977111117893"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.39997558519241921"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="darkGrid">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.249977111117893"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -2391,8 +2394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G2:BW49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R13" workbookViewId="0">
-      <selection activeCell="BK30" sqref="BK30"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="U29" sqref="U29"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -2450,7 +2453,7 @@
       <c r="BA2" s="15"/>
       <c r="BB2" s="15"/>
       <c r="BC2" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="BD2" s="15"/>
       <c r="BE2" s="15"/>
@@ -2576,27 +2579,27 @@
       <c r="AI4" s="15"/>
       <c r="AJ4" s="15"/>
       <c r="AK4" s="15" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="AL4" s="15" t="s">
         <v>1</v>
       </c>
       <c r="AM4" s="15" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="AN4" s="15"/>
       <c r="AO4" s="15" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AP4" s="15" t="s">
         <v>2</v>
       </c>
       <c r="AQ4" s="15" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="AR4" s="15"/>
       <c r="AS4" s="15" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="AT4" s="15"/>
       <c r="AU4" s="15"/>
@@ -2604,7 +2607,7 @@
       <c r="AW4" s="15"/>
       <c r="AX4" s="15"/>
       <c r="AY4" s="15" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AZ4" s="15"/>
       <c r="BA4" s="15"/>
@@ -2752,29 +2755,29 @@
       </c>
       <c r="AL6" s="15"/>
       <c r="AM6" s="15" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="AN6" s="15" t="s">
         <v>10</v>
       </c>
       <c r="AO6" s="15" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="AP6" s="15"/>
       <c r="AQ6" s="15" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="AR6" s="15" t="s">
         <v>11</v>
       </c>
       <c r="AS6" s="15" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="AT6" s="15" t="s">
         <v>12</v>
       </c>
       <c r="AU6" s="15" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="AV6" s="15" t="s">
         <v>13</v>
@@ -2786,7 +2789,7 @@
         <v>14</v>
       </c>
       <c r="AY6" s="15" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="AZ6" s="15" t="s">
         <v>15</v>
@@ -2798,7 +2801,7 @@
         <v>16</v>
       </c>
       <c r="BC6" s="15" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="BD6" s="15"/>
       <c r="BE6" s="15"/>
@@ -2930,27 +2933,27 @@
       <c r="AI8" s="15"/>
       <c r="AJ8" s="15"/>
       <c r="AK8" s="15" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="AL8" s="15"/>
       <c r="AM8" s="15" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="AN8" s="15" t="s">
         <v>21</v>
       </c>
       <c r="AO8" s="15" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="AP8" s="15" t="s">
         <v>22</v>
       </c>
       <c r="AQ8" s="15" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="AR8" s="15"/>
       <c r="AS8" s="15" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="AT8" s="15"/>
       <c r="AU8" s="15"/>
@@ -2958,7 +2961,7 @@
       <c r="AW8" s="15"/>
       <c r="AX8" s="15"/>
       <c r="AY8" s="15" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AZ8" s="15"/>
       <c r="BA8" s="15"/>
@@ -3094,17 +3097,17 @@
       <c r="AI10" s="15"/>
       <c r="AJ10" s="15"/>
       <c r="AK10" s="15" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="AL10" s="15"/>
       <c r="AM10" s="15" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="AN10" s="15" t="s">
         <v>27</v>
       </c>
       <c r="AO10" s="15" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="AP10" s="15"/>
       <c r="AQ10" s="15"/>
@@ -3157,19 +3160,27 @@
       <c r="P11" s="15"/>
       <c r="Q11" s="15"/>
       <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
+      <c r="S11" s="15" t="s">
+        <v>412</v>
+      </c>
       <c r="T11" s="15"/>
       <c r="U11" s="15"/>
       <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
+      <c r="W11" s="15" t="s">
+        <v>413</v>
+      </c>
       <c r="X11" s="15"/>
       <c r="Y11" s="15"/>
       <c r="Z11" s="15"/>
-      <c r="AA11" s="15"/>
+      <c r="AA11" s="15" t="s">
+        <v>419</v>
+      </c>
       <c r="AB11" s="15"/>
       <c r="AC11" s="15"/>
       <c r="AD11" s="15"/>
-      <c r="AE11" s="15"/>
+      <c r="AE11" s="15" t="s">
+        <v>419</v>
+      </c>
       <c r="AF11" s="15"/>
       <c r="AG11" s="15"/>
       <c r="AH11" s="15"/>
@@ -3238,25 +3249,25 @@
       <c r="Q12" s="15"/>
       <c r="R12" s="15"/>
       <c r="S12" s="15" t="s">
-        <v>414</v>
+        <v>24</v>
       </c>
       <c r="T12" s="15"/>
       <c r="U12" s="15"/>
       <c r="V12" s="15"/>
       <c r="W12" s="15" t="s">
-        <v>415</v>
+        <v>24</v>
       </c>
       <c r="X12" s="15"/>
       <c r="Y12" s="15"/>
       <c r="Z12" s="15"/>
       <c r="AA12" s="15" t="s">
-        <v>421</v>
+        <v>24</v>
       </c>
       <c r="AB12" s="15"/>
       <c r="AC12" s="15"/>
       <c r="AD12" s="15"/>
       <c r="AE12" s="15" t="s">
-        <v>421</v>
+        <v>0</v>
       </c>
       <c r="AF12" s="15"/>
       <c r="AG12" s="15"/>
@@ -3264,17 +3275,17 @@
       <c r="AI12" s="15"/>
       <c r="AJ12" s="15"/>
       <c r="AK12" s="15" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AL12" s="15" t="s">
         <v>35</v>
       </c>
       <c r="AM12" s="15" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AN12" s="15"/>
       <c r="AO12" s="15" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="AP12" s="15" t="s">
         <v>36</v>
@@ -3286,7 +3297,7 @@
         <v>37</v>
       </c>
       <c r="AS12" s="15" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="AT12" s="15"/>
       <c r="AU12" s="15"/>
@@ -3336,19 +3347,19 @@
       <c r="Q13" s="15"/>
       <c r="R13" s="15"/>
       <c r="S13" s="15" t="s">
-        <v>24</v>
+        <v>411</v>
       </c>
       <c r="T13" s="15"/>
       <c r="U13" s="15"/>
       <c r="V13" s="15"/>
       <c r="W13" s="15" t="s">
-        <v>24</v>
+        <v>412</v>
       </c>
       <c r="X13" s="15"/>
       <c r="Y13" s="15"/>
       <c r="Z13" s="15"/>
       <c r="AA13" s="15" t="s">
-        <v>24</v>
+        <v>413</v>
       </c>
       <c r="AB13" s="15"/>
       <c r="AC13" s="15"/>
@@ -3426,19 +3437,19 @@
       <c r="Q14" s="15"/>
       <c r="R14" s="15"/>
       <c r="S14" s="15" t="s">
-        <v>413</v>
+        <v>0</v>
       </c>
       <c r="T14" s="15"/>
       <c r="U14" s="15"/>
       <c r="V14" s="15"/>
       <c r="W14" s="15" t="s">
-        <v>414</v>
+        <v>0</v>
       </c>
       <c r="X14" s="15"/>
       <c r="Y14" s="15"/>
       <c r="Z14" s="15"/>
       <c r="AA14" s="15" t="s">
-        <v>415</v>
+        <v>0</v>
       </c>
       <c r="AB14" s="15"/>
       <c r="AC14" s="15"/>
@@ -3452,19 +3463,19 @@
       <c r="AI14" s="15"/>
       <c r="AJ14" s="15"/>
       <c r="AK14" s="15" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="AL14" s="15" t="s">
         <v>46</v>
       </c>
       <c r="AM14" s="15" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="AN14" s="15" t="s">
         <v>47</v>
       </c>
       <c r="AO14" s="15" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="AP14" s="15"/>
       <c r="AQ14" s="15"/>
@@ -3518,23 +3529,35 @@
       <c r="O15" s="15"/>
       <c r="P15" s="15"/>
       <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
+      <c r="R15" s="15" t="s">
+        <v>409</v>
+      </c>
       <c r="S15" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="T15" s="15"/>
+        <v>408</v>
+      </c>
+      <c r="T15" s="15" t="s">
+        <v>410</v>
+      </c>
       <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
+      <c r="V15" s="15" t="s">
+        <v>415</v>
+      </c>
       <c r="W15" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="X15" s="15"/>
+        <v>414</v>
+      </c>
+      <c r="X15" s="15" t="s">
+        <v>416</v>
+      </c>
       <c r="Y15" s="15"/>
-      <c r="Z15" s="15"/>
+      <c r="Z15" s="15" t="s">
+        <v>421</v>
+      </c>
       <c r="AA15" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="15"/>
+        <v>420</v>
+      </c>
+      <c r="AB15" s="15" t="s">
+        <v>422</v>
+      </c>
       <c r="AC15" s="15"/>
       <c r="AD15" s="15"/>
       <c r="AE15" s="15" t="s">
@@ -3562,13 +3585,13 @@
       <c r="AW15" s="15"/>
       <c r="AX15" s="15"/>
       <c r="AY15" s="15" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="AZ15" s="15"/>
       <c r="BA15" s="15"/>
       <c r="BB15" s="15"/>
       <c r="BC15" s="15" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="BD15" s="15"/>
       <c r="BE15" s="15"/>
@@ -3602,35 +3625,23 @@
       <c r="O16" s="15"/>
       <c r="P16" s="15"/>
       <c r="Q16" s="15"/>
-      <c r="R16" s="15" t="s">
-        <v>411</v>
-      </c>
+      <c r="R16" s="15"/>
       <c r="S16" s="15" t="s">
-        <v>410</v>
-      </c>
-      <c r="T16" s="15" t="s">
-        <v>412</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T16" s="15"/>
       <c r="U16" s="15"/>
-      <c r="V16" s="15" t="s">
-        <v>417</v>
-      </c>
+      <c r="V16" s="15"/>
       <c r="W16" s="15" t="s">
-        <v>416</v>
-      </c>
-      <c r="X16" s="15" t="s">
-        <v>418</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="X16" s="15"/>
       <c r="Y16" s="15"/>
-      <c r="Z16" s="15" t="s">
-        <v>423</v>
-      </c>
+      <c r="Z16" s="15"/>
       <c r="AA16" s="15" t="s">
-        <v>422</v>
-      </c>
-      <c r="AB16" s="15" t="s">
-        <v>424</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AB16" s="15"/>
       <c r="AC16" s="15"/>
       <c r="AD16" s="15"/>
       <c r="AE16" s="15" t="s">
@@ -3698,27 +3709,39 @@
       <c r="O17" s="15"/>
       <c r="P17" s="15"/>
       <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
+      <c r="R17" s="15" t="s">
+        <v>406</v>
+      </c>
       <c r="S17" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="T17" s="15"/>
+        <v>404</v>
+      </c>
+      <c r="T17" s="15" t="s">
+        <v>407</v>
+      </c>
       <c r="U17" s="15"/>
-      <c r="V17" s="15"/>
+      <c r="V17" s="15" t="s">
+        <v>418</v>
+      </c>
       <c r="W17" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="X17" s="15"/>
+        <v>417</v>
+      </c>
+      <c r="X17" s="15" t="s">
+        <v>418</v>
+      </c>
       <c r="Y17" s="15"/>
-      <c r="Z17" s="15"/>
+      <c r="Z17" s="15" t="s">
+        <v>424</v>
+      </c>
       <c r="AA17" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="15"/>
+        <v>423</v>
+      </c>
+      <c r="AB17" s="15" t="s">
+        <v>425</v>
+      </c>
       <c r="AC17" s="15"/>
       <c r="AD17" s="15"/>
       <c r="AE17" s="15" t="s">
-        <v>0</v>
+        <v>426</v>
       </c>
       <c r="AF17" s="15"/>
       <c r="AG17" s="15"/>
@@ -3734,7 +3757,7 @@
       <c r="AQ17" s="15"/>
       <c r="AR17" s="15"/>
       <c r="AS17" s="15" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="AT17" s="15" t="s">
         <v>55</v>
@@ -3752,7 +3775,7 @@
         <v>57</v>
       </c>
       <c r="AY17" s="15" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="AZ17" s="15"/>
       <c r="BA17" s="15"/>
@@ -3792,40 +3815,20 @@
       <c r="O18" s="15"/>
       <c r="P18" s="15"/>
       <c r="Q18" s="15"/>
-      <c r="R18" s="15" t="s">
-        <v>408</v>
-      </c>
-      <c r="S18" s="15" t="s">
-        <v>406</v>
-      </c>
-      <c r="T18" s="15" t="s">
-        <v>409</v>
-      </c>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="15"/>
       <c r="U18" s="15"/>
-      <c r="V18" s="15" t="s">
-        <v>420</v>
-      </c>
-      <c r="W18" s="15" t="s">
-        <v>419</v>
-      </c>
-      <c r="X18" s="15" t="s">
-        <v>420</v>
-      </c>
+      <c r="V18" s="15"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="15"/>
       <c r="Y18" s="15"/>
-      <c r="Z18" s="15" t="s">
-        <v>426</v>
-      </c>
-      <c r="AA18" s="15" t="s">
-        <v>425</v>
-      </c>
-      <c r="AB18" s="15" t="s">
-        <v>427</v>
-      </c>
+      <c r="Z18" s="15"/>
+      <c r="AA18" s="15"/>
+      <c r="AB18" s="15"/>
       <c r="AC18" s="15"/>
       <c r="AD18" s="15"/>
-      <c r="AE18" s="15" t="s">
-        <v>428</v>
-      </c>
+      <c r="AE18" s="15"/>
       <c r="AF18" s="15"/>
       <c r="AG18" s="15"/>
       <c r="AH18" s="15"/>
@@ -3881,14 +3884,16 @@
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
       <c r="M19" s="15" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="N19" s="15"/>
       <c r="O19" s="15"/>
       <c r="P19" s="15"/>
       <c r="Q19" s="15"/>
       <c r="R19" s="15"/>
-      <c r="S19" s="15"/>
+      <c r="S19" s="15" t="s">
+        <v>404</v>
+      </c>
       <c r="T19" s="15"/>
       <c r="U19" s="15"/>
       <c r="V19" s="15"/>
@@ -3948,7 +3953,7 @@
       <c r="BV19" s="16"/>
       <c r="BW19" s="16"/>
     </row>
-    <row r="20" spans="7:75" ht="24" customHeight="1">
+    <row r="20" spans="7:75" ht="24" customHeight="1" thickBot="1">
       <c r="G20" s="18"/>
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
@@ -3963,8 +3968,8 @@
       <c r="P20" s="15"/>
       <c r="Q20" s="15"/>
       <c r="R20" s="15"/>
-      <c r="S20" s="15" t="s">
-        <v>406</v>
+      <c r="S20" s="22" t="s">
+        <v>8</v>
       </c>
       <c r="T20" s="15"/>
       <c r="U20" s="15"/>
@@ -4028,13 +4033,13 @@
     <row r="21" spans="7:75" ht="24" customHeight="1">
       <c r="G21" s="16"/>
       <c r="H21" s="15" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I21" s="15" t="s">
         <v>0</v>
       </c>
       <c r="J21" s="15" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="K21" s="15" t="s">
         <v>0</v>
@@ -4043,7 +4048,7 @@
         <v>0</v>
       </c>
       <c r="M21" s="15" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="N21" s="15" t="s">
         <v>0</v>
@@ -4061,7 +4066,7 @@
         <v>0</v>
       </c>
       <c r="S21" s="15" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="T21" s="15" t="s">
         <v>0</v>
@@ -4097,7 +4102,7 @@
         <v>0</v>
       </c>
       <c r="AE21" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="AF21" s="15"/>
       <c r="AG21" s="15"/>
@@ -4254,7 +4259,7 @@
       <c r="AL23" s="15"/>
       <c r="AM23" s="15"/>
       <c r="AO23" s="17" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="AP23" s="17" t="s">
         <v>63</v>
@@ -4278,13 +4283,13 @@
         <v>66</v>
       </c>
       <c r="AW23" s="17" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="AZ23" s="15"/>
       <c r="BA23" s="15"/>
       <c r="BB23" s="15"/>
       <c r="BC23" s="15" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="BD23" s="15"/>
       <c r="BE23" s="15"/>
@@ -4292,7 +4297,7 @@
       <c r="BG23" s="15"/>
       <c r="BH23" s="15"/>
       <c r="BI23" s="15" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="BJ23" s="15"/>
       <c r="BK23" s="15"/>
@@ -4314,7 +4319,7 @@
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
       <c r="J24" s="15" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="K24" s="15" t="s">
         <v>0</v>
@@ -4323,7 +4328,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="15" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="N24" s="15" t="s">
         <v>0</v>
@@ -4332,7 +4337,7 @@
         <v>0</v>
       </c>
       <c r="P24" s="15" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="Q24" s="15" t="s">
         <v>0</v>
@@ -4341,7 +4346,7 @@
         <v>0</v>
       </c>
       <c r="S24" s="15" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="T24" s="15" t="s">
         <v>0</v>
@@ -4350,7 +4355,7 @@
         <v>0</v>
       </c>
       <c r="V24" s="15" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="W24" s="15"/>
       <c r="X24" s="15"/>
@@ -4361,7 +4366,7 @@
       <c r="AC24" s="15"/>
       <c r="AD24" s="15"/>
       <c r="AE24" s="15" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="AF24" s="15"/>
       <c r="AG24" s="15"/>
@@ -4438,19 +4443,19 @@
       <c r="AA25" s="15"/>
       <c r="AB25" s="15"/>
       <c r="AC25" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AD25" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AE25" s="15" t="s">
         <v>0</v>
       </c>
       <c r="AF25" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AG25" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AH25" s="15"/>
       <c r="AI25" s="15"/>
@@ -4462,28 +4467,28 @@
         <v>0</v>
       </c>
       <c r="AQ25" s="17" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AR25" s="17" t="s">
         <v>71</v>
       </c>
       <c r="AS25" s="17" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="AT25" s="17" t="s">
         <v>72</v>
       </c>
       <c r="AU25" s="17" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="AW25" s="17" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AX25" s="17" t="s">
         <v>73</v>
       </c>
       <c r="AY25" s="17" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AZ25" s="15"/>
       <c r="BA25" s="15"/>
@@ -4493,7 +4498,7 @@
       </c>
       <c r="BD25" s="15"/>
       <c r="BE25" s="15" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="BF25" s="15" t="s">
         <v>75</v>
@@ -4505,13 +4510,13 @@
         <v>76</v>
       </c>
       <c r="BI25" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="BJ25" s="15" t="s">
         <v>77</v>
       </c>
       <c r="BK25" s="15" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="BL25" s="15"/>
       <c r="BM25" s="15"/>
@@ -4558,19 +4563,19 @@
       <c r="AA26" s="15"/>
       <c r="AB26" s="15"/>
       <c r="AC26" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AD26" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AE26" s="15" t="s">
         <v>0</v>
       </c>
       <c r="AF26" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AG26" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AH26" s="15"/>
       <c r="AI26" s="15"/>
@@ -4619,12 +4624,12 @@
       <c r="BV26" s="16"/>
       <c r="BW26" s="16"/>
     </row>
-    <row r="27" spans="7:75" ht="24" customHeight="1">
+    <row r="27" spans="7:75" ht="24" customHeight="1" thickBot="1">
       <c r="G27" s="18"/>
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
       <c r="J27" s="15" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="K27" s="15" t="s">
         <v>0</v>
@@ -4642,7 +4647,7 @@
         <v>0</v>
       </c>
       <c r="P27" s="15" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="Q27" s="15" t="s">
         <v>0</v>
@@ -4650,8 +4655,8 @@
       <c r="R27" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="S27" s="15" t="s">
-        <v>295</v>
+      <c r="S27" s="22" t="s">
+        <v>293</v>
       </c>
       <c r="T27" s="15" t="s">
         <v>0</v>
@@ -4660,7 +4665,7 @@
         <v>0</v>
       </c>
       <c r="V27" s="15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="W27" s="15" t="s">
         <v>0</v>
@@ -4678,7 +4683,7 @@
         <v>0</v>
       </c>
       <c r="AB27" s="15" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AC27" s="15" t="s">
         <v>0</v>
@@ -4696,7 +4701,7 @@
         <v>0</v>
       </c>
       <c r="AH27" s="15" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="AI27" s="15" t="s">
         <v>0</v>
@@ -4717,64 +4722,64 @@
         <v>85</v>
       </c>
       <c r="AO27" s="17" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AQ27" s="17" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="AR27" s="17" t="s">
         <v>86</v>
       </c>
       <c r="AS27" s="17" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="AT27" s="17" t="s">
         <v>87</v>
       </c>
       <c r="AU27" s="17" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="AV27" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="AW27" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="AX27" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="AW27" s="17" t="s">
-        <v>313</v>
-      </c>
-      <c r="AX27" s="17" t="s">
+      <c r="AY27" s="17" t="s">
+        <v>323</v>
+      </c>
+      <c r="AZ27" s="15" t="s">
         <v>89</v>
-      </c>
-      <c r="AY27" s="17" t="s">
-        <v>325</v>
-      </c>
-      <c r="AZ27" s="15" t="s">
-        <v>90</v>
       </c>
       <c r="BA27" s="15" t="s">
         <v>0</v>
       </c>
       <c r="BB27" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="BC27" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="BD27" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="BC27" s="15" t="s">
-        <v>326</v>
-      </c>
-      <c r="BD27" s="15" t="s">
+      <c r="BE27" s="15" t="s">
+        <v>448</v>
+      </c>
+      <c r="BF27" s="15" t="s">
         <v>92</v>
-      </c>
-      <c r="BE27" s="15" t="s">
-        <v>450</v>
-      </c>
-      <c r="BF27" s="15" t="s">
-        <v>93</v>
       </c>
       <c r="BG27" s="15" t="s">
         <v>0</v>
       </c>
       <c r="BH27" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BI27" s="15" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="BJ27" s="15"/>
       <c r="BK27" s="15"/>
@@ -4786,7 +4791,7 @@
       <c r="BQ27" s="15"/>
       <c r="BR27" s="16"/>
       <c r="BS27" s="16" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="BT27" s="16"/>
       <c r="BU27" s="16"/>
@@ -4807,7 +4812,7 @@
       <c r="Q28" s="15"/>
       <c r="R28" s="15"/>
       <c r="S28" s="15" t="s">
-        <v>266</v>
+        <v>8</v>
       </c>
       <c r="T28" s="15"/>
       <c r="U28" s="15"/>
@@ -4819,19 +4824,19 @@
       <c r="AA28" s="15"/>
       <c r="AB28" s="15"/>
       <c r="AC28" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AD28" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AE28" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AF28" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AG28" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AH28" s="15"/>
       <c r="AI28" s="15"/>
@@ -4840,25 +4845,25 @@
       <c r="AL28" s="15"/>
       <c r="AM28" s="15"/>
       <c r="AO28" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ28" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="AQ28" s="17" t="s">
+      <c r="AS28" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU28" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="AS28" s="17" t="s">
+      <c r="AW28" s="17" t="s">
         <v>97</v>
-      </c>
-      <c r="AU28" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="AW28" s="17" t="s">
-        <v>99</v>
       </c>
       <c r="AZ28" s="15"/>
       <c r="BA28" s="15"/>
       <c r="BB28" s="15"/>
       <c r="BC28" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="BD28" s="15"/>
       <c r="BE28" s="15"/>
@@ -4866,7 +4871,7 @@
       <c r="BG28" s="15"/>
       <c r="BH28" s="15"/>
       <c r="BI28" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="BJ28" s="15"/>
       <c r="BK28" s="15"/>
@@ -4874,21 +4879,21 @@
       <c r="BM28" s="15"/>
       <c r="BN28" s="15"/>
       <c r="BO28" s="15" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="BP28" s="15" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="BQ28" s="15"/>
       <c r="BR28" s="16"/>
       <c r="BS28" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="BT28" s="16"/>
       <c r="BU28" s="16"/>
       <c r="BV28" s="16"/>
       <c r="BW28" s="16" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="29" spans="7:75" ht="24" customHeight="1">
@@ -4899,14 +4904,16 @@
       <c r="K29" s="15"/>
       <c r="L29" s="15"/>
       <c r="M29" s="15" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="N29" s="15"/>
       <c r="O29" s="15"/>
       <c r="P29" s="15"/>
       <c r="Q29" s="15"/>
       <c r="R29" s="15"/>
-      <c r="S29" s="15"/>
+      <c r="S29" s="15" t="s">
+        <v>264</v>
+      </c>
       <c r="T29" s="15"/>
       <c r="U29" s="15"/>
       <c r="V29" s="15"/>
@@ -4917,19 +4924,19 @@
       <c r="AA29" s="15"/>
       <c r="AB29" s="15"/>
       <c r="AC29" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AD29" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AE29" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AF29" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AG29" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AH29" s="15"/>
       <c r="AI29" s="15"/>
@@ -4941,13 +4948,13 @@
         <v>0</v>
       </c>
       <c r="AQ29" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="AS29" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="AU29" s="17" t="s">
         <v>304</v>
-      </c>
-      <c r="AS29" s="17" t="s">
-        <v>305</v>
-      </c>
-      <c r="AU29" s="17" t="s">
-        <v>306</v>
       </c>
       <c r="AW29" s="17" t="s">
         <v>0</v>
@@ -4956,7 +4963,7 @@
       <c r="BA29" s="15"/>
       <c r="BB29" s="15"/>
       <c r="BC29" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="BD29" s="15"/>
       <c r="BE29" s="15"/>
@@ -4964,41 +4971,41 @@
       <c r="BG29" s="15"/>
       <c r="BH29" s="15"/>
       <c r="BI29" s="15" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="BJ29" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="BK29" s="15" t="s">
         <v>0</v>
       </c>
       <c r="BL29" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="BM29" s="15" t="s">
         <v>0</v>
       </c>
       <c r="BN29" s="15" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="BO29" s="15" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="BP29" s="15" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="BQ29" s="15"/>
       <c r="BR29" s="16"/>
       <c r="BS29" s="16" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="BT29" s="16"/>
       <c r="BU29" s="16"/>
       <c r="BV29" s="16" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="BW29" s="16" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="30" spans="7:75" ht="24" customHeight="1">
@@ -5038,16 +5045,16 @@
       <c r="AL30" s="15"/>
       <c r="AM30" s="15"/>
       <c r="AO30" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AW30" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AZ30" s="15"/>
       <c r="BA30" s="15"/>
       <c r="BB30" s="15"/>
       <c r="BC30" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="BD30" s="15"/>
       <c r="BE30" s="15"/>
@@ -5085,13 +5092,13 @@
       <c r="P31" s="15"/>
       <c r="Q31" s="15"/>
       <c r="R31" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="S31" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="T31" s="15" t="s">
         <v>267</v>
-      </c>
-      <c r="S31" s="15" t="s">
-        <v>268</v>
-      </c>
-      <c r="T31" s="15" t="s">
-        <v>269</v>
       </c>
       <c r="U31" s="15"/>
       <c r="V31" s="15"/>
@@ -5101,7 +5108,7 @@
       <c r="Z31" s="15"/>
       <c r="AA31" s="15"/>
       <c r="AB31" s="15" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AC31" s="15"/>
       <c r="AD31" s="15"/>
@@ -5115,31 +5122,31 @@
       <c r="AL31" s="15"/>
       <c r="AM31" s="15"/>
       <c r="AO31" s="17" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AP31" s="17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AQ31" s="17" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AR31" s="17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AS31" s="17" t="s">
         <v>0</v>
       </c>
       <c r="AT31" s="17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AU31" s="17" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AV31" s="17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="AW31" s="17" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="AZ31" s="15"/>
       <c r="BA31" s="15"/>
@@ -5211,16 +5218,16 @@
       <c r="AL32" s="15"/>
       <c r="AM32" s="15"/>
       <c r="AQ32" s="17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="AU32" s="17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="AZ32" s="15"/>
       <c r="BA32" s="15"/>
       <c r="BB32" s="15"/>
       <c r="BC32" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="BD32" s="15"/>
       <c r="BE32" s="15"/>
@@ -5258,13 +5265,13 @@
       <c r="P33" s="15"/>
       <c r="Q33" s="15"/>
       <c r="R33" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="S33" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="T33" s="15" t="s">
         <v>270</v>
-      </c>
-      <c r="S33" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="T33" s="15" t="s">
-        <v>272</v>
       </c>
       <c r="U33" s="15"/>
       <c r="V33" s="15"/>
@@ -5288,25 +5295,25 @@
       <c r="AL33" s="15"/>
       <c r="AM33" s="15"/>
       <c r="AQ33" s="17" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AR33" s="17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AS33" s="17" t="s">
         <v>0</v>
       </c>
       <c r="AT33" s="17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AU33" s="17" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="AZ33" s="15"/>
       <c r="BA33" s="15"/>
       <c r="BB33" s="15"/>
       <c r="BC33" s="15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="BD33" s="15"/>
       <c r="BE33" s="15"/>
@@ -5383,7 +5390,7 @@
       <c r="BA34" s="15"/>
       <c r="BB34" s="15"/>
       <c r="BC34" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="BD34" s="15"/>
       <c r="BE34" s="15"/>
@@ -5421,13 +5428,13 @@
       <c r="P35" s="15"/>
       <c r="Q35" s="15"/>
       <c r="R35" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="S35" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="T35" s="15" t="s">
         <v>273</v>
-      </c>
-      <c r="S35" s="15" t="s">
-        <v>274</v>
-      </c>
-      <c r="T35" s="15" t="s">
-        <v>275</v>
       </c>
       <c r="U35" s="15"/>
       <c r="V35" s="15"/>
@@ -5452,11 +5459,11 @@
       <c r="AM35" s="15"/>
       <c r="AN35" s="15"/>
       <c r="AO35" s="15" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AP35" s="15"/>
       <c r="AQ35" s="15" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="AR35" s="15"/>
       <c r="AS35" s="15"/>
@@ -5470,19 +5477,19 @@
       <c r="BA35" s="15"/>
       <c r="BB35" s="15"/>
       <c r="BC35" s="15" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="BD35" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="BE35" s="15" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="BF35" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="BG35" s="15" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="BH35" s="15"/>
       <c r="BI35" s="15"/>
@@ -5563,11 +5570,11 @@
       <c r="BA36" s="15"/>
       <c r="BB36" s="15"/>
       <c r="BC36" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="BD36" s="15"/>
       <c r="BE36" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="BF36" s="15"/>
       <c r="BG36" s="15"/>
@@ -5600,18 +5607,18 @@
       </c>
       <c r="N37" s="15"/>
       <c r="O37" s="15" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="P37" s="15"/>
       <c r="Q37" s="15"/>
       <c r="R37" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="S37" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="T37" s="15" t="s">
         <v>276</v>
-      </c>
-      <c r="S37" s="15" t="s">
-        <v>277</v>
-      </c>
-      <c r="T37" s="15" t="s">
-        <v>278</v>
       </c>
       <c r="U37" s="15"/>
       <c r="V37" s="15"/>
@@ -5636,11 +5643,11 @@
       <c r="AM37" s="15"/>
       <c r="AN37" s="15"/>
       <c r="AO37" s="15" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="AP37" s="15"/>
       <c r="AQ37" s="15" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="AR37" s="15"/>
       <c r="AS37" s="15"/>
@@ -5654,13 +5661,13 @@
       <c r="BA37" s="15"/>
       <c r="BB37" s="15"/>
       <c r="BC37" s="15" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="BD37" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="BE37" s="15" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="BF37" s="15"/>
       <c r="BG37" s="15"/>
@@ -5737,7 +5744,7 @@
       <c r="BA38" s="15"/>
       <c r="BB38" s="15"/>
       <c r="BC38" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="BD38" s="15"/>
       <c r="BE38" s="15"/>
@@ -5772,18 +5779,18 @@
       </c>
       <c r="N39" s="15"/>
       <c r="O39" s="15" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="P39" s="15"/>
       <c r="Q39" s="15"/>
       <c r="R39" s="15" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="S39" s="15" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="T39" s="15" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="U39" s="15"/>
       <c r="V39" s="15"/>
@@ -5808,7 +5815,7 @@
       <c r="AM39" s="15"/>
       <c r="AN39" s="15"/>
       <c r="AO39" s="15" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AP39" s="15" t="s">
         <v>0</v>
@@ -5820,7 +5827,7 @@
         <v>0</v>
       </c>
       <c r="AS39" s="15" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="AT39" s="15"/>
       <c r="AU39" s="15"/>
@@ -5907,7 +5914,7 @@
       <c r="AQ40" s="15"/>
       <c r="AR40" s="15"/>
       <c r="AS40" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AT40" s="15"/>
       <c r="AU40" s="15"/>
@@ -5919,7 +5926,7 @@
       <c r="BA40" s="15"/>
       <c r="BB40" s="15"/>
       <c r="BC40" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="BD40" s="15"/>
       <c r="BE40" s="15"/>
@@ -5954,18 +5961,18 @@
       </c>
       <c r="N41" s="15"/>
       <c r="O41" s="15" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="P41" s="15"/>
       <c r="Q41" s="15"/>
       <c r="R41" s="15" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="S41" s="15" t="s">
         <v>0</v>
       </c>
       <c r="T41" s="15" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="U41" s="15"/>
       <c r="V41" s="15"/>
@@ -5990,11 +5997,11 @@
       <c r="AM41" s="15"/>
       <c r="AN41" s="15"/>
       <c r="AO41" s="15" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="AP41" s="15"/>
       <c r="AQ41" s="15" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="AR41" s="15"/>
       <c r="AS41" s="15" t="s">
@@ -6010,7 +6017,7 @@
       <c r="BA41" s="15"/>
       <c r="BB41" s="15"/>
       <c r="BC41" s="15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="BD41" s="15"/>
       <c r="BE41" s="15"/>
@@ -6079,7 +6086,7 @@
       </c>
       <c r="AR42" s="15"/>
       <c r="AS42" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="AT42" s="15"/>
       <c r="AU42" s="15"/>
@@ -6091,7 +6098,7 @@
       <c r="BA42" s="15"/>
       <c r="BB42" s="15"/>
       <c r="BC42" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="BD42" s="15"/>
       <c r="BE42" s="15"/>
@@ -6122,7 +6129,7 @@
       <c r="K43" s="15"/>
       <c r="L43" s="15"/>
       <c r="M43" s="15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="N43" s="15" t="s">
         <v>0</v>
@@ -6149,7 +6156,7 @@
         <v>0</v>
       </c>
       <c r="V43" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="W43" s="15"/>
       <c r="X43" s="15"/>
@@ -6174,13 +6181,13 @@
       <c r="AO43" s="15"/>
       <c r="AP43" s="15"/>
       <c r="AQ43" s="15" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="AR43" s="15" t="s">
         <v>0</v>
       </c>
       <c r="AS43" s="15" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="AT43" s="15"/>
       <c r="AU43" s="15"/>
@@ -6192,7 +6199,7 @@
       <c r="BA43" s="15"/>
       <c r="BB43" s="15"/>
       <c r="BC43" s="15" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="BD43" s="15"/>
       <c r="BE43" s="15"/>
@@ -6269,7 +6276,7 @@
       <c r="BA44" s="15"/>
       <c r="BB44" s="15"/>
       <c r="BC44" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="BD44" s="15"/>
       <c r="BE44" s="15"/>
@@ -6346,7 +6353,7 @@
       <c r="BA45" s="15"/>
       <c r="BB45" s="15"/>
       <c r="BC45" s="15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="BD45" s="15"/>
       <c r="BE45" s="15"/>
@@ -6354,13 +6361,13 @@
       <c r="BG45" s="15"/>
       <c r="BH45" s="15"/>
       <c r="BI45" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="BJ45" s="15"/>
       <c r="BK45" s="15"/>
       <c r="BL45" s="15"/>
       <c r="BM45" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="BN45" s="15"/>
       <c r="BO45" s="15"/>
@@ -6390,7 +6397,7 @@
       <c r="T46" s="15"/>
       <c r="U46" s="15"/>
       <c r="V46" s="15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="W46" s="15" t="s">
         <v>0</v>
@@ -6408,7 +6415,7 @@
         <v>0</v>
       </c>
       <c r="AB46" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="AC46" s="15"/>
       <c r="AD46" s="15"/>
@@ -6437,7 +6444,7 @@
       <c r="BA46" s="15"/>
       <c r="BB46" s="15"/>
       <c r="BC46" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="BD46" s="15"/>
       <c r="BE46" s="15"/>
@@ -6445,13 +6452,13 @@
       <c r="BG46" s="15"/>
       <c r="BH46" s="15"/>
       <c r="BI46" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="BJ46" s="15"/>
       <c r="BK46" s="15"/>
       <c r="BL46" s="15"/>
       <c r="BM46" s="15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="BN46" s="15"/>
       <c r="BO46" s="15"/>
@@ -6513,37 +6520,37 @@
       <c r="BA47" s="15"/>
       <c r="BB47" s="15"/>
       <c r="BC47" s="15" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="BD47" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="BE47" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="BF47" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="BE47" s="15" t="s">
+      <c r="BG47" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="BF47" s="15" t="s">
+      <c r="BH47" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="BG47" s="15" t="s">
+      <c r="BI47" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="BH47" s="15" t="s">
+      <c r="BJ47" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="BI47" s="15" t="s">
+      <c r="BK47" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="BJ47" s="15" t="s">
+      <c r="BL47" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="BK47" s="15" t="s">
+      <c r="BM47" s="15" t="s">
         <v>145</v>
-      </c>
-      <c r="BL47" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="BM47" s="15" t="s">
-        <v>147</v>
       </c>
       <c r="BN47" s="15"/>
       <c r="BO47" s="15"/>
@@ -6611,13 +6618,13 @@
       <c r="BG48" s="15"/>
       <c r="BH48" s="15"/>
       <c r="BI48" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="BJ48" s="15"/>
       <c r="BK48" s="15"/>
       <c r="BL48" s="15"/>
       <c r="BM48" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="BN48" s="15"/>
       <c r="BO48" s="15"/>
@@ -6685,13 +6692,13 @@
       <c r="BG49" s="15"/>
       <c r="BH49" s="15"/>
       <c r="BI49" s="15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="BJ49" s="15"/>
       <c r="BK49" s="15"/>
       <c r="BL49" s="15"/>
       <c r="BM49" s="15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="BN49" s="15"/>
       <c r="BO49" s="15"/>
@@ -6706,29 +6713,29 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="beginsWith" dxfId="12" priority="2" operator="beginsWith" text="|">
-      <formula>LEFT(A1,LEN("|"))="|"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="11" priority="5" operator="beginsWith" text="OT">
-      <formula>LEFT(A1,LEN("OT"))="OT"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="10" priority="6" operator="beginsWith" text="HQ">
-      <formula>LEFT(A1,LEN("HQ"))="HQ"</formula>
-    </cfRule>
-    <cfRule type="containsBlanks" dxfId="9" priority="9">
-      <formula>LEN(TRIM(A1))=0</formula>
-    </cfRule>
     <cfRule type="beginsWith" dxfId="6" priority="1" operator="beginsWith" text="FO">
       <formula>LEFT(A1,LEN("FO"))="FO"</formula>
     </cfRule>
+    <cfRule type="beginsWith" dxfId="5" priority="2" operator="beginsWith" text="|">
+      <formula>LEFT(A1,LEN("|"))="|"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="4" priority="5" operator="beginsWith" text="OT">
+      <formula>LEFT(A1,LEN("OT"))="OT"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="6" operator="beginsWith" text="HQ">
+      <formula>LEFT(A1,LEN("HQ"))="HQ"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="2" priority="9">
+      <formula>LEN(TRIM(A1))=0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="beginsWith" dxfId="8" priority="4" operator="beginsWith" text="CT">
+    <cfRule type="beginsWith" dxfId="1" priority="4" operator="beginsWith" text="CT">
       <formula>LEFT(A1,LEN("CT"))="CT"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="beginsWith" dxfId="7" priority="3" operator="beginsWith" text="AP">
+    <cfRule type="beginsWith" dxfId="0" priority="3" operator="beginsWith" text="AP">
       <formula>LEFT(A1,LEN("AP"))="AP"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6745,10 +6752,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C986"/>
+  <dimension ref="A1:E986"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
     <sheetView topLeftCell="A24" workbookViewId="1">
       <selection activeCell="C24" sqref="C24"/>
@@ -6759,325 +6766,364 @@
     <col min="1" max="1" width="7.1640625" style="9" customWidth="1"/>
     <col min="2" max="2" width="42.6640625" style="20" customWidth="1"/>
     <col min="3" max="3" width="93.33203125" style="7" customWidth="1"/>
-    <col min="4" max="16384" width="17.33203125" hidden="1"/>
+    <col min="4" max="4" width="37.83203125" style="28" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" style="24" customWidth="1"/>
+    <col min="6" max="16384" width="17.33203125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="48" customHeight="1">
+    <row r="1" spans="1:5" ht="48" customHeight="1">
       <c r="A1" s="8" t="str">
         <f t="shared" ref="A1:A9" si="0">CONCATENATE("HQ", ROW())</f>
         <v>HQ1</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="48" customHeight="1">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="48" customHeight="1">
       <c r="A2" s="8" t="str">
         <f t="shared" si="0"/>
         <v>HQ2</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="48" customHeight="1">
+        <v>153</v>
+      </c>
+      <c r="D2" s="25"/>
+    </row>
+    <row r="3" spans="1:5" ht="48" customHeight="1">
       <c r="A3" s="8" t="str">
         <f t="shared" si="0"/>
         <v>HQ3</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="96" customHeight="1">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="96" customHeight="1">
       <c r="A4" s="8" t="str">
         <f t="shared" si="0"/>
         <v>HQ4</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="96" customHeight="1">
+        <v>157</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="96" customHeight="1">
       <c r="A5" s="8" t="str">
         <f t="shared" si="0"/>
         <v>HQ5</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="48" customHeight="1">
+        <v>159</v>
+      </c>
+      <c r="D5" s="25"/>
+    </row>
+    <row r="6" spans="1:5" ht="48" customHeight="1">
       <c r="A6" s="8" t="str">
         <f t="shared" si="0"/>
         <v>HQ6</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="48" customHeight="1">
+        <v>161</v>
+      </c>
+      <c r="D6" s="25"/>
+    </row>
+    <row r="7" spans="1:5" ht="48" customHeight="1">
       <c r="A7" s="8" t="str">
         <f t="shared" si="0"/>
         <v>HQ7</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" ht="48" customHeight="1">
+      <c r="D7" s="25"/>
+    </row>
+    <row r="8" spans="1:5" ht="48" customHeight="1">
       <c r="A8" s="8" t="str">
         <f t="shared" si="0"/>
         <v>HQ8</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="48" customHeight="1">
+        <v>164</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>468</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="48" customHeight="1">
       <c r="A9" s="8" t="str">
         <f t="shared" si="0"/>
         <v>HQ9</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" ht="48" customHeight="1">
+      <c r="D9" s="25" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="48" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="19"/>
       <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:3" ht="48" customHeight="1">
+      <c r="D10" s="25"/>
+    </row>
+    <row r="11" spans="1:5" ht="48" customHeight="1">
       <c r="A11" s="8" t="str">
         <f t="shared" ref="A11:A16" si="1">CONCATENATE("BK", ROW()-10)</f>
         <v>BK1</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C11" s="12"/>
-    </row>
-    <row r="12" spans="1:3" ht="48" customHeight="1">
+      <c r="D11" s="26"/>
+    </row>
+    <row r="12" spans="1:5" ht="48" customHeight="1">
       <c r="A12" s="8" t="str">
         <f t="shared" si="1"/>
         <v>BK2</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" ht="48" customHeight="1">
+      <c r="D12" s="25"/>
+    </row>
+    <row r="13" spans="1:5" ht="48" customHeight="1">
       <c r="A13" s="8" t="str">
         <f t="shared" si="1"/>
         <v>BK3</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:3" ht="48" customHeight="1">
+      <c r="D13" s="25"/>
+    </row>
+    <row r="14" spans="1:5" ht="48" customHeight="1">
       <c r="A14" s="8" t="str">
         <f t="shared" si="1"/>
         <v>BK4</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:3" ht="48" customHeight="1">
+      <c r="D14" s="25"/>
+    </row>
+    <row r="15" spans="1:5" ht="48" customHeight="1">
       <c r="A15" s="8" t="str">
         <f t="shared" si="1"/>
         <v>BK5</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:3" ht="48" customHeight="1">
+      <c r="D15" s="27"/>
+    </row>
+    <row r="16" spans="1:5" ht="48" customHeight="1">
       <c r="A16" s="8" t="str">
         <f t="shared" si="1"/>
         <v>BK6</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:3" ht="48" customHeight="1">
+      <c r="D16" s="25"/>
+    </row>
+    <row r="17" spans="1:4" ht="48" customHeight="1">
       <c r="A17" s="14"/>
       <c r="B17" s="19"/>
       <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="1:3" ht="48" customHeight="1">
+      <c r="D17" s="27"/>
+    </row>
+    <row r="18" spans="1:4" ht="48" customHeight="1">
       <c r="A18" s="14"/>
       <c r="B18" s="19"/>
       <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3" ht="48" customHeight="1">
+      <c r="D18" s="27"/>
+    </row>
+    <row r="19" spans="1:4" ht="48" customHeight="1">
       <c r="A19" s="14" t="str">
         <f t="shared" ref="A19:A32" si="2">CONCATENATE("OT", ROW()-18)</f>
         <v>OT1</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C19" s="6"/>
-    </row>
-    <row r="20" spans="1:3" ht="48" customHeight="1">
+      <c r="D19" s="27"/>
+    </row>
+    <row r="20" spans="1:4" ht="48" customHeight="1">
       <c r="A20" s="14" t="str">
         <f t="shared" si="2"/>
         <v>OT2</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="1:3" ht="48" customHeight="1">
+      <c r="D20" s="25"/>
+    </row>
+    <row r="21" spans="1:4" ht="48" customHeight="1">
       <c r="A21" s="14" t="str">
         <f t="shared" si="2"/>
         <v>OT3</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="1:3" ht="48" customHeight="1">
+      <c r="D21" s="25"/>
+    </row>
+    <row r="22" spans="1:4" ht="48" customHeight="1">
       <c r="A22" s="14" t="str">
         <f t="shared" si="2"/>
         <v>OT4</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="48" customHeight="1">
+        <v>447</v>
+      </c>
+      <c r="D22" s="25"/>
+    </row>
+    <row r="23" spans="1:4" ht="48" customHeight="1">
       <c r="A23" s="14" t="str">
         <f t="shared" si="2"/>
         <v>OT5</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="48" customHeight="1">
+        <v>447</v>
+      </c>
+      <c r="D23" s="25"/>
+    </row>
+    <row r="24" spans="1:4" ht="48" customHeight="1">
       <c r="A24" s="14" t="str">
         <f t="shared" si="2"/>
         <v>OT6</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="1:3" ht="48" customHeight="1">
+      <c r="D24" s="25"/>
+    </row>
+    <row r="25" spans="1:4" ht="48" customHeight="1">
       <c r="A25" s="14" t="str">
         <f t="shared" si="2"/>
         <v>OT7</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="1:3" ht="48" customHeight="1">
+      <c r="D25" s="25"/>
+    </row>
+    <row r="26" spans="1:4" ht="48" customHeight="1">
       <c r="A26" s="14" t="str">
         <f t="shared" si="2"/>
         <v>OT8</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="1:3" ht="48" customHeight="1">
+      <c r="D26" s="25"/>
+    </row>
+    <row r="27" spans="1:4" ht="48" customHeight="1">
       <c r="A27" s="14" t="str">
         <f t="shared" si="2"/>
         <v>OT9</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C27" s="5"/>
-    </row>
-    <row r="28" spans="1:3" ht="48" customHeight="1">
+      <c r="D27" s="25"/>
+    </row>
+    <row r="28" spans="1:4" ht="48" customHeight="1">
       <c r="A28" s="14" t="str">
         <f t="shared" si="2"/>
         <v>OT10</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="48" customHeight="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="48" customHeight="1">
       <c r="A29" s="14" t="str">
         <f t="shared" si="2"/>
         <v>OT11</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="48" customHeight="1">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="48" customHeight="1">
       <c r="A30" s="14" t="str">
         <f t="shared" si="2"/>
         <v>OT12</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="48" customHeight="1">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="48" customHeight="1">
       <c r="A31" s="14" t="str">
         <f t="shared" si="2"/>
         <v>OT13</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="48" customHeight="1">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="48" customHeight="1">
       <c r="A32" s="14" t="str">
         <f t="shared" si="2"/>
         <v>OT14</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="48" customHeight="1">
@@ -10825,193 +10871,193 @@
   <sheetData>
     <row r="1" spans="1:3" ht="48" customHeight="1">
       <c r="A1" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="47" customHeight="1">
       <c r="A2" s="10" t="str">
-        <f>CONCATENATE("CT", ROW() - MATCH("CT1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" ref="A2:A16" si="0">CONCATENATE("CT", ROW() - MATCH("CT1",$A$1:$A$130,0) +1)</f>
         <v>CT2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="47" customHeight="1">
       <c r="A3" s="10" t="str">
-        <f>CONCATENATE("CT", ROW() - MATCH("CT1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="0"/>
         <v>CT3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="47" customHeight="1">
       <c r="A4" s="10" t="str">
-        <f>CONCATENATE("CT", ROW() - MATCH("CT1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="0"/>
         <v>CT4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="47" customHeight="1">
       <c r="A5" s="10" t="str">
-        <f>CONCATENATE("CT", ROW() - MATCH("CT1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="0"/>
         <v>CT5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="47" customHeight="1">
       <c r="A6" s="10" t="str">
-        <f>CONCATENATE("CT", ROW() - MATCH("CT1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="0"/>
         <v>CT6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="47" customHeight="1">
       <c r="A7" s="10" t="str">
-        <f>CONCATENATE("CT", ROW() - MATCH("CT1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="0"/>
         <v>CT7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="47" customHeight="1">
       <c r="A8" s="10" t="str">
-        <f>CONCATENATE("CT", ROW() - MATCH("CT1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="0"/>
         <v>CT8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="47" customHeight="1">
       <c r="A9" s="10" t="str">
-        <f>CONCATENATE("CT", ROW() - MATCH("CT1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="0"/>
         <v>CT9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="47" customHeight="1">
       <c r="A10" s="10" t="str">
-        <f>CONCATENATE("CT", ROW() - MATCH("CT1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="0"/>
         <v>CT10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="47" customHeight="1">
       <c r="A11" s="10" t="str">
-        <f>CONCATENATE("CT", ROW() - MATCH("CT1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="0"/>
         <v>CT11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="47" customHeight="1">
       <c r="A12" s="10" t="str">
-        <f>CONCATENATE("CT", ROW() - MATCH("CT1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="0"/>
         <v>CT12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="47" customHeight="1">
       <c r="A13" s="10" t="str">
-        <f>CONCATENATE("CT", ROW() - MATCH("CT1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="0"/>
         <v>CT13</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="47" customHeight="1">
       <c r="A14" s="10" t="str">
-        <f>CONCATENATE("CT", ROW() - MATCH("CT1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="0"/>
         <v>CT14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="47" customHeight="1">
       <c r="A15" s="10" t="str">
-        <f>CONCATENATE("CT", ROW() - MATCH("CT1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="0"/>
         <v>CT15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="47" customHeight="1">
       <c r="A16" s="10" t="str">
-        <f>CONCATENATE("CT", ROW() - MATCH("CT1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="0"/>
         <v>CT16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="47" customHeight="1">
@@ -11026,205 +11072,205 @@
     </row>
     <row r="19" spans="1:3" ht="96" customHeight="1">
       <c r="A19" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="47" customHeight="1">
       <c r="A20" s="14" t="str">
-        <f>CONCATENATE("AP", ROW() - MATCH("AP1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" ref="A20:A35" si="1">CONCATENATE("AP", ROW() - MATCH("AP1",$A$1:$A$130,0) +1)</f>
         <v>AP2</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>230</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="47" customHeight="1">
       <c r="A21" s="14" t="str">
-        <f>CONCATENATE("AP", ROW() - MATCH("AP1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="1"/>
         <v>AP3</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="47" customHeight="1">
       <c r="A22" s="14" t="str">
-        <f>CONCATENATE("AP", ROW() - MATCH("AP1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="1"/>
         <v>AP4</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="47" customHeight="1">
       <c r="A23" s="14" t="str">
-        <f>CONCATENATE("AP", ROW() - MATCH("AP1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="1"/>
         <v>AP5</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="47" customHeight="1">
       <c r="A24" s="14" t="str">
-        <f>CONCATENATE("AP", ROW() - MATCH("AP1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="1"/>
         <v>AP6</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="47" customHeight="1">
       <c r="A25" s="14" t="str">
-        <f>CONCATENATE("AP", ROW() - MATCH("AP1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="1"/>
         <v>AP7</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="47" customHeight="1">
       <c r="A26" s="14" t="str">
-        <f>CONCATENATE("AP", ROW() - MATCH("AP1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="1"/>
         <v>AP8</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="47" customHeight="1">
       <c r="A27" s="14" t="str">
-        <f>CONCATENATE("AP", ROW() - MATCH("AP1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="1"/>
         <v>AP9</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="47" customHeight="1">
       <c r="A28" s="14" t="str">
-        <f>CONCATENATE("AP", ROW() - MATCH("AP1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="1"/>
         <v>AP10</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="47" customHeight="1">
       <c r="A29" s="14" t="str">
-        <f>CONCATENATE("AP", ROW() - MATCH("AP1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="1"/>
         <v>AP11</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="47" customHeight="1">
       <c r="A30" s="14" t="str">
-        <f>CONCATENATE("AP", ROW() - MATCH("AP1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="1"/>
         <v>AP12</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="47" customHeight="1">
       <c r="A31" s="14" t="str">
-        <f>CONCATENATE("AP", ROW() - MATCH("AP1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="1"/>
         <v>AP13</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="47" customHeight="1">
       <c r="A32" s="14" t="str">
-        <f>CONCATENATE("AP", ROW() - MATCH("AP1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="1"/>
         <v>AP14</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="47" customHeight="1">
       <c r="A33" s="14" t="str">
-        <f>CONCATENATE("AP", ROW() - MATCH("AP1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="1"/>
         <v>AP15</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="47" customHeight="1">
       <c r="A34" s="14" t="str">
-        <f>CONCATENATE("AP", ROW() - MATCH("AP1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="1"/>
         <v>AP16</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="47" customHeight="1">
       <c r="A35" s="14" t="str">
-        <f>CONCATENATE("AP", ROW() - MATCH("AP1",$A$1:$A$130,0) +1)</f>
+        <f t="shared" si="1"/>
         <v>AP17</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="47" customHeight="1">
@@ -11239,215 +11285,215 @@
     </row>
     <row r="38" spans="1:3" ht="47" customHeight="1">
       <c r="A38" s="14" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C38" s="5"/>
     </row>
     <row r="39" spans="1:3" ht="47" customHeight="1">
       <c r="A39" s="14" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="5"/>
     </row>
     <row r="40" spans="1:3" ht="47" customHeight="1">
       <c r="A40" s="14" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C40" s="5"/>
     </row>
     <row r="41" spans="1:3" ht="47" customHeight="1">
       <c r="A41" s="14" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C41" s="5"/>
     </row>
     <row r="42" spans="1:3" ht="47" customHeight="1">
       <c r="A42" s="14" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C42" s="5"/>
     </row>
     <row r="43" spans="1:3" ht="47" customHeight="1">
       <c r="A43" s="14" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C43" s="5"/>
     </row>
     <row r="44" spans="1:3" ht="47" customHeight="1">
       <c r="A44" s="14" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C44" s="5"/>
     </row>
     <row r="45" spans="1:3" ht="47" customHeight="1">
       <c r="A45" s="14" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C45" s="5"/>
     </row>
     <row r="46" spans="1:3" ht="47" customHeight="1">
       <c r="A46" s="14" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C46" s="5"/>
     </row>
     <row r="47" spans="1:3" ht="47" customHeight="1">
       <c r="A47" s="14" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C47" s="5"/>
     </row>
     <row r="48" spans="1:3" ht="47" customHeight="1">
       <c r="A48" s="14" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C48" s="5"/>
     </row>
     <row r="49" spans="1:3" ht="47" customHeight="1">
       <c r="A49" s="14" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C49" s="5"/>
     </row>
     <row r="50" spans="1:3" ht="47" customHeight="1">
       <c r="A50" s="14" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C50" s="5"/>
     </row>
     <row r="51" spans="1:3" ht="47" customHeight="1">
       <c r="A51" s="14" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C51" s="5"/>
     </row>
     <row r="52" spans="1:3" ht="47" customHeight="1">
       <c r="A52" s="14" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C52" s="5"/>
     </row>
     <row r="53" spans="1:3" ht="47" customHeight="1">
       <c r="A53" s="14" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C53" s="5"/>
     </row>
     <row r="54" spans="1:3" ht="47" customHeight="1">
       <c r="A54" s="14" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C54" s="5"/>
     </row>
     <row r="55" spans="1:3" ht="47" customHeight="1">
       <c r="A55" s="14" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C55" s="5"/>
     </row>
     <row r="56" spans="1:3" ht="47" customHeight="1">
       <c r="A56" s="14" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B56" s="21" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C56" s="5"/>
     </row>
     <row r="57" spans="1:3" ht="47" customHeight="1">
       <c r="A57" s="14" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C57" s="5"/>
     </row>
     <row r="58" spans="1:3" ht="47" customHeight="1">
       <c r="A58" s="14" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C58" s="5"/>
     </row>
     <row r="59" spans="1:3" ht="47" customHeight="1">
       <c r="A59" s="14" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C59" s="5"/>
     </row>
     <row r="60" spans="1:3" ht="47" customHeight="1">
       <c r="A60" s="14" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C60" s="5"/>
     </row>
     <row r="61" spans="1:3" ht="47" customHeight="1">
       <c r="A61" s="14" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C61" s="5"/>
     </row>
@@ -11473,13 +11519,13 @@
     </row>
     <row r="66" spans="1:3" ht="47" customHeight="1">
       <c r="A66" s="14" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="47" customHeight="1">
@@ -11488,10 +11534,10 @@
         <v>SW2</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="47" customHeight="1">
@@ -11500,10 +11546,10 @@
         <v>SW3</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="47" customHeight="1">
@@ -11512,10 +11558,10 @@
         <v>SW4</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="47" customHeight="1">
@@ -15376,7 +15422,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -15407,631 +15452,630 @@
   <sheetData>
     <row r="1" spans="1:2" ht="48" customHeight="1">
       <c r="A1" s="8" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="48" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="48" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="48" customHeight="1">
       <c r="A4" s="8" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="48" customHeight="1">
       <c r="A5" s="8" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="48" customHeight="1">
       <c r="A6" s="8" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="48" customHeight="1">
       <c r="A7" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="48" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="48" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="48" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="48" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="48" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="48" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="48" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="48" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="48" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="48" customHeight="1">
       <c r="A17" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="48" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="48" customHeight="1">
       <c r="A19" s="8" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="48" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="48" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="48" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="48" customHeight="1">
       <c r="A23" s="8" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="48" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="48" customHeight="1">
       <c r="A25" s="8" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="48" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="48" customHeight="1">
       <c r="A29" s="8" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="48" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="48" customHeight="1">
       <c r="A31" s="8" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="48" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="48" customHeight="1">
       <c r="A33" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="B33" s="19" t="s">
         <v>452</v>
-      </c>
-      <c r="B33" s="19" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="48" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="48" customHeight="1">
       <c r="A35" s="8" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="48" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="48" customHeight="1">
       <c r="A37" s="8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="48" customHeight="1">
       <c r="A38" s="8" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="48" customHeight="1">
       <c r="A39" s="8" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="48" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="48" customHeight="1">
       <c r="A41" s="8" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="48" customHeight="1">
       <c r="A45" s="8" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="48" customHeight="1">
       <c r="A46" s="8" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="48" customHeight="1">
       <c r="A47" s="8" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="48" customHeight="1">
       <c r="A48" s="8" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="48" customHeight="1">
       <c r="A49" s="8" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="48" customHeight="1">
       <c r="A50" s="8" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="48" customHeight="1">
       <c r="A51" s="8" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="48" customHeight="1">
       <c r="A54" s="8" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="48" customHeight="1">
       <c r="A55" s="8" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="48" customHeight="1">
       <c r="A56" s="8" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="48" customHeight="1">
       <c r="A57" s="8" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="48" customHeight="1">
       <c r="A58" s="8" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="48" customHeight="1">
       <c r="A59" s="8" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="48" customHeight="1">
       <c r="A60" s="8" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="48" customHeight="1">
       <c r="A61" s="8" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="48" customHeight="1">
       <c r="A62" s="8" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="48" customHeight="1">
       <c r="A63" s="8" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B63" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="48" customHeight="1">
       <c r="A64" s="8" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="48" customHeight="1">
       <c r="A65" s="8" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="48" customHeight="1">
       <c r="A66" s="8" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="48" customHeight="1">
       <c r="A67" s="8" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="48" customHeight="1">
       <c r="A68" s="8" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="48" customHeight="1">
       <c r="A69" s="8" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="48" customHeight="1">
       <c r="A70" s="8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="48" customHeight="1">
       <c r="A71" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="48" customHeight="1">
       <c r="A72" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="48" customHeight="1">
       <c r="A73" s="8" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="48" customHeight="1">
       <c r="A74" s="8" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B74" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="48" customHeight="1">
       <c r="A75" s="8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B75" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="48" customHeight="1">
       <c r="A76" s="8" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B76" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="48" customHeight="1">
       <c r="A77" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="48" customHeight="1">
       <c r="A78" s="8" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B78" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="48" customHeight="1">
       <c r="A79" s="8" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B79" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="48" customHeight="1">
       <c r="A80" s="8" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B80" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="48" customHeight="1">
       <c r="A81" s="8" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B81" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="48" customHeight="1">
       <c r="A82" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="B82" s="19" t="s">
         <v>464</v>
-      </c>
-      <c r="B82" s="19" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="48" customHeight="1">
       <c r="A83" s="8" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B83" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="48" customHeight="1">
       <c r="A84" s="8" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B84" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="48" customHeight="1">
       <c r="A85" s="8" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B85" s="19" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
started state machine and event system.
</commit_message>
<xml_diff>
--- a/stories/colddeadwater/data/map.xlsx
+++ b/stories/colddeadwater/data/map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500"/>
-    <workbookView xWindow="10720" yWindow="0" windowWidth="27680" windowHeight="21080" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="1120" yWindow="0" windowWidth="37280" windowHeight="21080" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="world" sheetId="1" r:id="rId1"/>
@@ -2394,8 +2394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G2:BW49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="U29" sqref="U29"/>
+    <sheetView tabSelected="1" topLeftCell="N18" workbookViewId="0">
+      <selection activeCell="AO43" sqref="AO43:AO45"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>

</xml_diff>

<commit_message>
cleaned up states more
</commit_message>
<xml_diff>
--- a/stories/colddeadwater/data/map.xlsx
+++ b/stories/colddeadwater/data/map.xlsx
@@ -4,8 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500"/>
-    <workbookView xWindow="1120" yWindow="0" windowWidth="37280" windowHeight="21080" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="world" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="463">
   <si>
     <t>.</t>
   </si>
@@ -475,99 +474,27 @@
     <t>G8</t>
   </si>
   <si>
-    <t>Survivors Camp West</t>
-  </si>
-  <si>
     <t>You are surrounded by tents.</t>
   </si>
   <si>
-    <t>Survivors Camp</t>
-  </si>
-  <si>
     <t>You are surrounded by tents. Mothers and children huddled around fires stare at you with lifeless eyes. There are more tents to the east and west, and headquarters is to the south.</t>
   </si>
   <si>
-    <t>Survivors Camp East</t>
-  </si>
-  <si>
     <t>You are surrounded by tents.</t>
   </si>
   <si>
-    <t>Munitions Depot</t>
-  </si>
-  <si>
     <t>You are in the center of a cluster of three buildings. The arms locker is here, guarded by an extremely large man with almost no neck. The mechanical shop is also here, littered with old tires and scrap metal. Finally, and most importantly, the food store is  here. A massive steel door with a combination lock guards this building. To the north is the survivors camp, to the east is headquarters, and to the south is the training ground.</t>
   </si>
   <si>
-    <t>Headquarters</t>
-  </si>
-  <si>
     <t>You are at HQ, which is a nice way of saying the middle of the junkyard. Large sheet metal walls surround the encampment on all sides. A desk made of old tires and plywood is set up nearby. Up the path to the &lt;em&gt;east&lt;/em&gt; is a lookout tower. To the &lt;em&gt;west&lt;/em&gt; lies a group of ramshackle buildings used to store food and munitions. To the &lt;em&gt;south&lt;/em&gt; is a large green medical tent. Finally, to the &lt;em&gt;north&lt;/em&gt; is a group of tents housing survivors, those too weak to pick up a gun and fight.</t>
   </si>
   <si>
-    <t>Gate</t>
-  </si>
-  <si>
     <t>The encampment gate is here, with a lookout tower.</t>
   </si>
   <si>
-    <t>Training Ground</t>
-  </si>
-  <si>
-    <t>Medical Tent</t>
-  </si>
-  <si>
     <t>You are in the medical tent. Filthy beds line the walls, most are occupied. It smells like death. You can see the tent door to the &lt;em&gt;north&lt;/em&gt;, which is the only exit.</t>
   </si>
   <si>
-    <t>Junk Pile</t>
-  </si>
-  <si>
-    <t>Underground Bunker</t>
-  </si>
-  <si>
-    <t>Underground Bunker</t>
-  </si>
-  <si>
-    <t>Underground Bunker</t>
-  </si>
-  <si>
-    <t>Underground Bunker</t>
-  </si>
-  <si>
-    <t>Underground Bunker</t>
-  </si>
-  <si>
-    <t>Underground Hideout</t>
-  </si>
-  <si>
-    <t>Outside The Gate</t>
-  </si>
-  <si>
-    <t>Outside The East Wall</t>
-  </si>
-  <si>
-    <t>Outside The South Wall</t>
-  </si>
-  <si>
-    <t>Outside The West Wall</t>
-  </si>
-  <si>
-    <t>Outside The West Wall</t>
-  </si>
-  <si>
-    <t>Rocky Path</t>
-  </si>
-  <si>
-    <t>Rocky Path</t>
-  </si>
-  <si>
-    <t>Duck Pond</t>
-  </si>
-  <si>
-    <t>Rocky Path</t>
-  </si>
-  <si>
     <t>Abandoned Highway</t>
   </si>
   <si>
@@ -1433,6 +1360,57 @@
   </si>
   <si>
     <t>fenton</t>
+  </si>
+  <si>
+    <t>the west end of the survivors camp</t>
+  </si>
+  <si>
+    <t>the survivors camp</t>
+  </si>
+  <si>
+    <t>the east end of the survivors camp</t>
+  </si>
+  <si>
+    <t>the munitions depot</t>
+  </si>
+  <si>
+    <t>the headquarters</t>
+  </si>
+  <si>
+    <t>the gate</t>
+  </si>
+  <si>
+    <t>the training ground</t>
+  </si>
+  <si>
+    <t>the medical tent</t>
+  </si>
+  <si>
+    <t>the junk pile</t>
+  </si>
+  <si>
+    <t>an underground hideout</t>
+  </si>
+  <si>
+    <t>a dusty tunnel</t>
+  </si>
+  <si>
+    <t>outside the gate</t>
+  </si>
+  <si>
+    <t>the eastern camp wall</t>
+  </si>
+  <si>
+    <t>the southern camp wall</t>
+  </si>
+  <si>
+    <t>a duck pond</t>
+  </si>
+  <si>
+    <t>the western camp wall</t>
+  </si>
+  <si>
+    <t>a rocky path</t>
   </si>
 </sst>
 </file>
@@ -1499,7 +1477,7 @@
       <name val="Menlo Regular"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1519,6 +1497,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1556,7 +1540,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="173">
+  <cellStyleXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1730,8 +1714,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1817,8 +1809,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="173">
+  <cellStyles count="181">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1905,6 +1900,10 @@
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1991,9 +1990,177 @@
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.249977111117893"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.249977111117893"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="0.39997558519241921"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkGrid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.249977111117893"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.249977111117893"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.249977111117893"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="0.39997558519241921"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="darkGrid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.249977111117893"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="9" tint="-0.249977111117893"/>
@@ -2394,10 +2561,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G2:BW49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N18" workbookViewId="0">
-      <selection activeCell="AO43" sqref="AO43:AO45"/>
+    <sheetView topLeftCell="B18" workbookViewId="0">
+      <selection activeCell="AX12" sqref="AX12"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -2453,7 +2619,7 @@
       <c r="BA2" s="15"/>
       <c r="BB2" s="15"/>
       <c r="BC2" s="15" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="BD2" s="15"/>
       <c r="BE2" s="15"/>
@@ -2579,27 +2745,27 @@
       <c r="AI4" s="15"/>
       <c r="AJ4" s="15"/>
       <c r="AK4" s="15" t="s">
-        <v>350</v>
+        <v>326</v>
       </c>
       <c r="AL4" s="15" t="s">
         <v>1</v>
       </c>
       <c r="AM4" s="15" t="s">
-        <v>351</v>
+        <v>327</v>
       </c>
       <c r="AN4" s="15"/>
       <c r="AO4" s="15" t="s">
-        <v>352</v>
+        <v>328</v>
       </c>
       <c r="AP4" s="15" t="s">
         <v>2</v>
       </c>
       <c r="AQ4" s="15" t="s">
-        <v>353</v>
+        <v>329</v>
       </c>
       <c r="AR4" s="15"/>
       <c r="AS4" s="15" t="s">
-        <v>354</v>
+        <v>330</v>
       </c>
       <c r="AT4" s="15"/>
       <c r="AU4" s="15"/>
@@ -2607,7 +2773,7 @@
       <c r="AW4" s="15"/>
       <c r="AX4" s="15"/>
       <c r="AY4" s="15" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="AZ4" s="15"/>
       <c r="BA4" s="15"/>
@@ -2755,29 +2921,29 @@
       </c>
       <c r="AL6" s="15"/>
       <c r="AM6" s="15" t="s">
-        <v>355</v>
+        <v>331</v>
       </c>
       <c r="AN6" s="15" t="s">
         <v>10</v>
       </c>
       <c r="AO6" s="15" t="s">
-        <v>356</v>
+        <v>332</v>
       </c>
       <c r="AP6" s="15"/>
       <c r="AQ6" s="15" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
       <c r="AR6" s="15" t="s">
         <v>11</v>
       </c>
       <c r="AS6" s="15" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="AT6" s="15" t="s">
         <v>12</v>
       </c>
       <c r="AU6" s="15" t="s">
-        <v>346</v>
+        <v>322</v>
       </c>
       <c r="AV6" s="15" t="s">
         <v>13</v>
@@ -2789,7 +2955,7 @@
         <v>14</v>
       </c>
       <c r="AY6" s="15" t="s">
-        <v>344</v>
+        <v>320</v>
       </c>
       <c r="AZ6" s="15" t="s">
         <v>15</v>
@@ -2801,7 +2967,7 @@
         <v>16</v>
       </c>
       <c r="BC6" s="15" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
       <c r="BD6" s="15"/>
       <c r="BE6" s="15"/>
@@ -2933,27 +3099,27 @@
       <c r="AI8" s="15"/>
       <c r="AJ8" s="15"/>
       <c r="AK8" s="15" t="s">
-        <v>359</v>
+        <v>335</v>
       </c>
       <c r="AL8" s="15"/>
       <c r="AM8" s="15" t="s">
-        <v>360</v>
+        <v>336</v>
       </c>
       <c r="AN8" s="15" t="s">
         <v>21</v>
       </c>
       <c r="AO8" s="15" t="s">
-        <v>361</v>
+        <v>337</v>
       </c>
       <c r="AP8" s="15" t="s">
         <v>22</v>
       </c>
       <c r="AQ8" s="15" t="s">
-        <v>362</v>
+        <v>338</v>
       </c>
       <c r="AR8" s="15"/>
       <c r="AS8" s="15" t="s">
-        <v>363</v>
+        <v>339</v>
       </c>
       <c r="AT8" s="15"/>
       <c r="AU8" s="15"/>
@@ -2961,7 +3127,7 @@
       <c r="AW8" s="15"/>
       <c r="AX8" s="15"/>
       <c r="AY8" s="15" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="AZ8" s="15"/>
       <c r="BA8" s="15"/>
@@ -3097,17 +3263,17 @@
       <c r="AI10" s="15"/>
       <c r="AJ10" s="15"/>
       <c r="AK10" s="15" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
       <c r="AL10" s="15"/>
       <c r="AM10" s="15" t="s">
-        <v>365</v>
+        <v>341</v>
       </c>
       <c r="AN10" s="15" t="s">
         <v>27</v>
       </c>
       <c r="AO10" s="15" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="AP10" s="15"/>
       <c r="AQ10" s="15"/>
@@ -3161,25 +3327,25 @@
       <c r="Q11" s="15"/>
       <c r="R11" s="15"/>
       <c r="S11" s="15" t="s">
-        <v>412</v>
+        <v>388</v>
       </c>
       <c r="T11" s="15"/>
       <c r="U11" s="15"/>
       <c r="V11" s="15"/>
       <c r="W11" s="15" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
       <c r="X11" s="15"/>
       <c r="Y11" s="15"/>
       <c r="Z11" s="15"/>
       <c r="AA11" s="15" t="s">
-        <v>419</v>
+        <v>395</v>
       </c>
       <c r="AB11" s="15"/>
       <c r="AC11" s="15"/>
       <c r="AD11" s="15"/>
       <c r="AE11" s="15" t="s">
-        <v>419</v>
+        <v>395</v>
       </c>
       <c r="AF11" s="15"/>
       <c r="AG11" s="15"/>
@@ -3275,17 +3441,17 @@
       <c r="AI12" s="15"/>
       <c r="AJ12" s="15"/>
       <c r="AK12" s="15" t="s">
-        <v>367</v>
+        <v>343</v>
       </c>
       <c r="AL12" s="15" t="s">
         <v>35</v>
       </c>
       <c r="AM12" s="15" t="s">
-        <v>368</v>
+        <v>344</v>
       </c>
       <c r="AN12" s="15"/>
       <c r="AO12" s="15" t="s">
-        <v>369</v>
+        <v>345</v>
       </c>
       <c r="AP12" s="15" t="s">
         <v>36</v>
@@ -3297,7 +3463,7 @@
         <v>37</v>
       </c>
       <c r="AS12" s="15" t="s">
-        <v>370</v>
+        <v>346</v>
       </c>
       <c r="AT12" s="15"/>
       <c r="AU12" s="15"/>
@@ -3347,19 +3513,19 @@
       <c r="Q13" s="15"/>
       <c r="R13" s="15"/>
       <c r="S13" s="15" t="s">
-        <v>411</v>
+        <v>387</v>
       </c>
       <c r="T13" s="15"/>
       <c r="U13" s="15"/>
       <c r="V13" s="15"/>
       <c r="W13" s="15" t="s">
-        <v>412</v>
+        <v>388</v>
       </c>
       <c r="X13" s="15"/>
       <c r="Y13" s="15"/>
       <c r="Z13" s="15"/>
       <c r="AA13" s="15" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
       <c r="AB13" s="15"/>
       <c r="AC13" s="15"/>
@@ -3463,19 +3629,19 @@
       <c r="AI14" s="15"/>
       <c r="AJ14" s="15"/>
       <c r="AK14" s="15" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="AL14" s="15" t="s">
         <v>46</v>
       </c>
       <c r="AM14" s="15" t="s">
-        <v>372</v>
+        <v>348</v>
       </c>
       <c r="AN14" s="15" t="s">
         <v>47</v>
       </c>
       <c r="AO14" s="15" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
       <c r="AP14" s="15"/>
       <c r="AQ14" s="15"/>
@@ -3530,33 +3696,33 @@
       <c r="P15" s="15"/>
       <c r="Q15" s="15"/>
       <c r="R15" s="15" t="s">
-        <v>409</v>
+        <v>385</v>
       </c>
       <c r="S15" s="15" t="s">
-        <v>408</v>
+        <v>384</v>
       </c>
       <c r="T15" s="15" t="s">
-        <v>410</v>
+        <v>386</v>
       </c>
       <c r="U15" s="15"/>
       <c r="V15" s="15" t="s">
-        <v>415</v>
+        <v>391</v>
       </c>
       <c r="W15" s="15" t="s">
-        <v>414</v>
+        <v>390</v>
       </c>
       <c r="X15" s="15" t="s">
-        <v>416</v>
+        <v>392</v>
       </c>
       <c r="Y15" s="15"/>
       <c r="Z15" s="15" t="s">
-        <v>421</v>
+        <v>397</v>
       </c>
       <c r="AA15" s="15" t="s">
-        <v>420</v>
+        <v>396</v>
       </c>
       <c r="AB15" s="15" t="s">
-        <v>422</v>
+        <v>398</v>
       </c>
       <c r="AC15" s="15"/>
       <c r="AD15" s="15"/>
@@ -3585,13 +3751,13 @@
       <c r="AW15" s="15"/>
       <c r="AX15" s="15"/>
       <c r="AY15" s="15" t="s">
-        <v>374</v>
+        <v>350</v>
       </c>
       <c r="AZ15" s="15"/>
       <c r="BA15" s="15"/>
       <c r="BB15" s="15"/>
       <c r="BC15" s="15" t="s">
-        <v>340</v>
+        <v>316</v>
       </c>
       <c r="BD15" s="15"/>
       <c r="BE15" s="15"/>
@@ -3710,38 +3876,38 @@
       <c r="P17" s="15"/>
       <c r="Q17" s="15"/>
       <c r="R17" s="15" t="s">
-        <v>406</v>
+        <v>382</v>
       </c>
       <c r="S17" s="15" t="s">
-        <v>404</v>
+        <v>380</v>
       </c>
       <c r="T17" s="15" t="s">
-        <v>407</v>
+        <v>383</v>
       </c>
       <c r="U17" s="15"/>
       <c r="V17" s="15" t="s">
-        <v>418</v>
+        <v>394</v>
       </c>
       <c r="W17" s="15" t="s">
-        <v>417</v>
+        <v>393</v>
       </c>
       <c r="X17" s="15" t="s">
-        <v>418</v>
+        <v>394</v>
       </c>
       <c r="Y17" s="15"/>
       <c r="Z17" s="15" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
       <c r="AA17" s="15" t="s">
-        <v>423</v>
+        <v>399</v>
       </c>
       <c r="AB17" s="15" t="s">
-        <v>425</v>
+        <v>401</v>
       </c>
       <c r="AC17" s="15"/>
       <c r="AD17" s="15"/>
       <c r="AE17" s="15" t="s">
-        <v>426</v>
+        <v>402</v>
       </c>
       <c r="AF17" s="15"/>
       <c r="AG17" s="15"/>
@@ -3757,7 +3923,7 @@
       <c r="AQ17" s="15"/>
       <c r="AR17" s="15"/>
       <c r="AS17" s="15" t="s">
-        <v>375</v>
+        <v>351</v>
       </c>
       <c r="AT17" s="15" t="s">
         <v>55</v>
@@ -3775,7 +3941,7 @@
         <v>57</v>
       </c>
       <c r="AY17" s="15" t="s">
-        <v>376</v>
+        <v>352</v>
       </c>
       <c r="AZ17" s="15"/>
       <c r="BA17" s="15"/>
@@ -3884,7 +4050,7 @@
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
       <c r="M19" s="15" t="s">
-        <v>281</v>
+        <v>257</v>
       </c>
       <c r="N19" s="15"/>
       <c r="O19" s="15"/>
@@ -3892,7 +4058,7 @@
       <c r="Q19" s="15"/>
       <c r="R19" s="15"/>
       <c r="S19" s="15" t="s">
-        <v>404</v>
+        <v>380</v>
       </c>
       <c r="T19" s="15"/>
       <c r="U19" s="15"/>
@@ -4033,13 +4199,13 @@
     <row r="21" spans="7:75" ht="24" customHeight="1">
       <c r="G21" s="16"/>
       <c r="H21" s="15" t="s">
-        <v>282</v>
+        <v>258</v>
       </c>
       <c r="I21" s="15" t="s">
         <v>0</v>
       </c>
       <c r="J21" s="15" t="s">
-        <v>283</v>
+        <v>259</v>
       </c>
       <c r="K21" s="15" t="s">
         <v>0</v>
@@ -4048,7 +4214,7 @@
         <v>0</v>
       </c>
       <c r="M21" s="15" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
       <c r="N21" s="15" t="s">
         <v>0</v>
@@ -4066,7 +4232,7 @@
         <v>0</v>
       </c>
       <c r="S21" s="15" t="s">
-        <v>285</v>
+        <v>261</v>
       </c>
       <c r="T21" s="15" t="s">
         <v>0</v>
@@ -4102,7 +4268,7 @@
         <v>0</v>
       </c>
       <c r="AE21" s="15" t="s">
-        <v>402</v>
+        <v>378</v>
       </c>
       <c r="AF21" s="15"/>
       <c r="AG21" s="15"/>
@@ -4259,7 +4425,7 @@
       <c r="AL23" s="15"/>
       <c r="AM23" s="15"/>
       <c r="AO23" s="17" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="AP23" s="17" t="s">
         <v>63</v>
@@ -4283,13 +4449,13 @@
         <v>66</v>
       </c>
       <c r="AW23" s="17" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="AZ23" s="15"/>
       <c r="BA23" s="15"/>
       <c r="BB23" s="15"/>
       <c r="BC23" s="15" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="BD23" s="15"/>
       <c r="BE23" s="15"/>
@@ -4297,7 +4463,7 @@
       <c r="BG23" s="15"/>
       <c r="BH23" s="15"/>
       <c r="BI23" s="15" t="s">
-        <v>377</v>
+        <v>353</v>
       </c>
       <c r="BJ23" s="15"/>
       <c r="BK23" s="15"/>
@@ -4319,7 +4485,7 @@
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
       <c r="J24" s="15" t="s">
-        <v>286</v>
+        <v>262</v>
       </c>
       <c r="K24" s="15" t="s">
         <v>0</v>
@@ -4328,7 +4494,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="15" t="s">
-        <v>287</v>
+        <v>263</v>
       </c>
       <c r="N24" s="15" t="s">
         <v>0</v>
@@ -4337,7 +4503,7 @@
         <v>0</v>
       </c>
       <c r="P24" s="15" t="s">
-        <v>288</v>
+        <v>264</v>
       </c>
       <c r="Q24" s="15" t="s">
         <v>0</v>
@@ -4346,7 +4512,7 @@
         <v>0</v>
       </c>
       <c r="S24" s="15" t="s">
-        <v>289</v>
+        <v>265</v>
       </c>
       <c r="T24" s="15" t="s">
         <v>0</v>
@@ -4355,7 +4521,7 @@
         <v>0</v>
       </c>
       <c r="V24" s="15" t="s">
-        <v>290</v>
+        <v>266</v>
       </c>
       <c r="W24" s="15"/>
       <c r="X24" s="15"/>
@@ -4366,7 +4532,7 @@
       <c r="AC24" s="15"/>
       <c r="AD24" s="15"/>
       <c r="AE24" s="15" t="s">
-        <v>401</v>
+        <v>377</v>
       </c>
       <c r="AF24" s="15"/>
       <c r="AG24" s="15"/>
@@ -4443,19 +4609,19 @@
       <c r="AA25" s="15"/>
       <c r="AB25" s="15"/>
       <c r="AC25" s="15" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="AD25" s="15" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="AE25" s="15" t="s">
         <v>0</v>
       </c>
       <c r="AF25" s="15" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="AG25" s="15" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="AH25" s="15"/>
       <c r="AI25" s="15"/>
@@ -4467,28 +4633,28 @@
         <v>0</v>
       </c>
       <c r="AQ25" s="17" t="s">
-        <v>296</v>
+        <v>272</v>
       </c>
       <c r="AR25" s="17" t="s">
         <v>71</v>
       </c>
       <c r="AS25" s="17" t="s">
-        <v>297</v>
+        <v>273</v>
       </c>
       <c r="AT25" s="17" t="s">
         <v>72</v>
       </c>
       <c r="AU25" s="17" t="s">
-        <v>298</v>
+        <v>274</v>
       </c>
       <c r="AW25" s="17" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
       <c r="AX25" s="17" t="s">
         <v>73</v>
       </c>
       <c r="AY25" s="17" t="s">
-        <v>322</v>
+        <v>298</v>
       </c>
       <c r="AZ25" s="15"/>
       <c r="BA25" s="15"/>
@@ -4498,7 +4664,7 @@
       </c>
       <c r="BD25" s="15"/>
       <c r="BE25" s="15" t="s">
-        <v>378</v>
+        <v>354</v>
       </c>
       <c r="BF25" s="15" t="s">
         <v>75</v>
@@ -4510,13 +4676,13 @@
         <v>76</v>
       </c>
       <c r="BI25" s="15" t="s">
-        <v>379</v>
+        <v>355</v>
       </c>
       <c r="BJ25" s="15" t="s">
         <v>77</v>
       </c>
       <c r="BK25" s="15" t="s">
-        <v>380</v>
+        <v>356</v>
       </c>
       <c r="BL25" s="15"/>
       <c r="BM25" s="15"/>
@@ -4563,19 +4729,19 @@
       <c r="AA26" s="15"/>
       <c r="AB26" s="15"/>
       <c r="AC26" s="15" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="AD26" s="15" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="AE26" s="15" t="s">
         <v>0</v>
       </c>
       <c r="AF26" s="15" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="AG26" s="15" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="AH26" s="15"/>
       <c r="AI26" s="15"/>
@@ -4589,9 +4755,12 @@
       <c r="AQ26" s="17" t="s">
         <v>79</v>
       </c>
+      <c r="AR26" s="29"/>
       <c r="AS26" s="17" t="s">
         <v>80</v>
       </c>
+      <c r="AT26" s="29"/>
+      <c r="AU26" s="29"/>
       <c r="AY26" s="17" t="s">
         <v>81</v>
       </c>
@@ -4629,7 +4798,7 @@
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
       <c r="J27" s="15" t="s">
-        <v>291</v>
+        <v>267</v>
       </c>
       <c r="K27" s="15" t="s">
         <v>0</v>
@@ -4647,7 +4816,7 @@
         <v>0</v>
       </c>
       <c r="P27" s="15" t="s">
-        <v>292</v>
+        <v>268</v>
       </c>
       <c r="Q27" s="15" t="s">
         <v>0</v>
@@ -4656,7 +4825,7 @@
         <v>0</v>
       </c>
       <c r="S27" s="22" t="s">
-        <v>293</v>
+        <v>269</v>
       </c>
       <c r="T27" s="15" t="s">
         <v>0</v>
@@ -4665,7 +4834,7 @@
         <v>0</v>
       </c>
       <c r="V27" s="15" t="s">
-        <v>294</v>
+        <v>270</v>
       </c>
       <c r="W27" s="15" t="s">
         <v>0</v>
@@ -4683,7 +4852,7 @@
         <v>0</v>
       </c>
       <c r="AB27" s="15" t="s">
-        <v>295</v>
+        <v>271</v>
       </c>
       <c r="AC27" s="15" t="s">
         <v>0</v>
@@ -4701,7 +4870,7 @@
         <v>0</v>
       </c>
       <c r="AH27" s="15" t="s">
-        <v>393</v>
+        <v>369</v>
       </c>
       <c r="AI27" s="15" t="s">
         <v>0</v>
@@ -4722,34 +4891,34 @@
         <v>85</v>
       </c>
       <c r="AO27" s="17" t="s">
-        <v>318</v>
+        <v>294</v>
       </c>
       <c r="AQ27" s="17" t="s">
-        <v>299</v>
+        <v>275</v>
       </c>
       <c r="AR27" s="17" t="s">
         <v>86</v>
       </c>
       <c r="AS27" s="17" t="s">
-        <v>300</v>
+        <v>276</v>
       </c>
       <c r="AT27" s="17" t="s">
         <v>87</v>
       </c>
       <c r="AU27" s="17" t="s">
-        <v>301</v>
+        <v>277</v>
       </c>
       <c r="AV27" s="17" t="s">
         <v>8</v>
       </c>
       <c r="AW27" s="17" t="s">
-        <v>311</v>
+        <v>287</v>
       </c>
       <c r="AX27" s="17" t="s">
         <v>88</v>
       </c>
       <c r="AY27" s="17" t="s">
-        <v>323</v>
+        <v>299</v>
       </c>
       <c r="AZ27" s="15" t="s">
         <v>89</v>
@@ -4761,13 +4930,13 @@
         <v>90</v>
       </c>
       <c r="BC27" s="15" t="s">
-        <v>324</v>
+        <v>300</v>
       </c>
       <c r="BD27" s="15" t="s">
         <v>91</v>
       </c>
       <c r="BE27" s="15" t="s">
-        <v>448</v>
+        <v>424</v>
       </c>
       <c r="BF27" s="15" t="s">
         <v>92</v>
@@ -4779,7 +4948,7 @@
         <v>93</v>
       </c>
       <c r="BI27" s="15" t="s">
-        <v>381</v>
+        <v>357</v>
       </c>
       <c r="BJ27" s="15"/>
       <c r="BK27" s="15"/>
@@ -4791,7 +4960,7 @@
       <c r="BQ27" s="15"/>
       <c r="BR27" s="16"/>
       <c r="BS27" s="16" t="s">
-        <v>388</v>
+        <v>364</v>
       </c>
       <c r="BT27" s="16"/>
       <c r="BU27" s="16"/>
@@ -4824,19 +4993,19 @@
       <c r="AA28" s="15"/>
       <c r="AB28" s="15"/>
       <c r="AC28" s="15" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="AD28" s="15" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="AE28" s="15" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="AF28" s="15" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="AG28" s="15" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="AH28" s="15"/>
       <c r="AI28" s="15"/>
@@ -4850,9 +5019,11 @@
       <c r="AQ28" s="17" t="s">
         <v>95</v>
       </c>
+      <c r="AR28" s="29"/>
       <c r="AS28" s="17" t="s">
         <v>8</v>
       </c>
+      <c r="AT28" s="29"/>
       <c r="AU28" s="17" t="s">
         <v>96</v>
       </c>
@@ -4879,10 +5050,10 @@
       <c r="BM28" s="15"/>
       <c r="BN28" s="15"/>
       <c r="BO28" s="15" t="s">
-        <v>386</v>
+        <v>362</v>
       </c>
       <c r="BP28" s="15" t="s">
-        <v>387</v>
+        <v>363</v>
       </c>
       <c r="BQ28" s="15"/>
       <c r="BR28" s="16"/>
@@ -4893,7 +5064,7 @@
       <c r="BU28" s="16"/>
       <c r="BV28" s="16"/>
       <c r="BW28" s="16" t="s">
-        <v>389</v>
+        <v>365</v>
       </c>
     </row>
     <row r="29" spans="7:75" ht="24" customHeight="1">
@@ -4904,7 +5075,7 @@
       <c r="K29" s="15"/>
       <c r="L29" s="15"/>
       <c r="M29" s="15" t="s">
-        <v>287</v>
+        <v>263</v>
       </c>
       <c r="N29" s="15"/>
       <c r="O29" s="15"/>
@@ -4912,7 +5083,7 @@
       <c r="Q29" s="15"/>
       <c r="R29" s="15"/>
       <c r="S29" s="15" t="s">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="T29" s="15"/>
       <c r="U29" s="15"/>
@@ -4924,19 +5095,19 @@
       <c r="AA29" s="15"/>
       <c r="AB29" s="15"/>
       <c r="AC29" s="15" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="AD29" s="15" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="AE29" s="15" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="AF29" s="15" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="AG29" s="15" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="AH29" s="15"/>
       <c r="AI29" s="15"/>
@@ -4948,13 +5119,15 @@
         <v>0</v>
       </c>
       <c r="AQ29" s="17" t="s">
-        <v>302</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="AR29" s="29"/>
       <c r="AS29" s="17" t="s">
-        <v>303</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="AT29" s="29"/>
       <c r="AU29" s="17" t="s">
-        <v>304</v>
+        <v>280</v>
       </c>
       <c r="AW29" s="17" t="s">
         <v>0</v>
@@ -4971,7 +5144,7 @@
       <c r="BG29" s="15"/>
       <c r="BH29" s="15"/>
       <c r="BI29" s="15" t="s">
-        <v>382</v>
+        <v>358</v>
       </c>
       <c r="BJ29" s="15" t="s">
         <v>102</v>
@@ -4986,26 +5159,26 @@
         <v>0</v>
       </c>
       <c r="BN29" s="15" t="s">
-        <v>451</v>
+        <v>427</v>
       </c>
       <c r="BO29" s="15" t="s">
-        <v>390</v>
+        <v>366</v>
       </c>
       <c r="BP29" s="15" t="s">
-        <v>391</v>
+        <v>367</v>
       </c>
       <c r="BQ29" s="15"/>
       <c r="BR29" s="16"/>
       <c r="BS29" s="16" t="s">
-        <v>391</v>
+        <v>367</v>
       </c>
       <c r="BT29" s="16"/>
       <c r="BU29" s="16"/>
       <c r="BV29" s="16" t="s">
-        <v>392</v>
+        <v>368</v>
       </c>
       <c r="BW29" s="16" t="s">
-        <v>388</v>
+        <v>364</v>
       </c>
     </row>
     <row r="30" spans="7:75" ht="24" customHeight="1">
@@ -5092,13 +5265,13 @@
       <c r="P31" s="15"/>
       <c r="Q31" s="15"/>
       <c r="R31" s="15" t="s">
-        <v>265</v>
+        <v>241</v>
       </c>
       <c r="S31" s="15" t="s">
-        <v>266</v>
+        <v>242</v>
       </c>
       <c r="T31" s="15" t="s">
-        <v>267</v>
+        <v>243</v>
       </c>
       <c r="U31" s="15"/>
       <c r="V31" s="15"/>
@@ -5108,7 +5281,7 @@
       <c r="Z31" s="15"/>
       <c r="AA31" s="15"/>
       <c r="AB31" s="15" t="s">
-        <v>295</v>
+        <v>271</v>
       </c>
       <c r="AC31" s="15"/>
       <c r="AD31" s="15"/>
@@ -5122,13 +5295,13 @@
       <c r="AL31" s="15"/>
       <c r="AM31" s="15"/>
       <c r="AO31" s="17" t="s">
-        <v>317</v>
+        <v>293</v>
       </c>
       <c r="AP31" s="17" t="s">
         <v>107</v>
       </c>
       <c r="AQ31" s="17" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
       <c r="AR31" s="17" t="s">
         <v>108</v>
@@ -5140,13 +5313,13 @@
         <v>109</v>
       </c>
       <c r="AU31" s="17" t="s">
-        <v>313</v>
+        <v>289</v>
       </c>
       <c r="AV31" s="17" t="s">
         <v>110</v>
       </c>
       <c r="AW31" s="17" t="s">
-        <v>312</v>
+        <v>288</v>
       </c>
       <c r="AZ31" s="15"/>
       <c r="BA31" s="15"/>
@@ -5265,13 +5438,13 @@
       <c r="P33" s="15"/>
       <c r="Q33" s="15"/>
       <c r="R33" s="15" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="S33" s="15" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
       <c r="T33" s="15" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="U33" s="15"/>
       <c r="V33" s="15"/>
@@ -5295,7 +5468,7 @@
       <c r="AL33" s="15"/>
       <c r="AM33" s="15"/>
       <c r="AQ33" s="17" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="AR33" s="17" t="s">
         <v>114</v>
@@ -5307,7 +5480,7 @@
         <v>115</v>
       </c>
       <c r="AU33" s="17" t="s">
-        <v>314</v>
+        <v>290</v>
       </c>
       <c r="AZ33" s="15"/>
       <c r="BA33" s="15"/>
@@ -5428,13 +5601,13 @@
       <c r="P35" s="15"/>
       <c r="Q35" s="15"/>
       <c r="R35" s="15" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
       <c r="S35" s="15" t="s">
-        <v>272</v>
+        <v>248</v>
       </c>
       <c r="T35" s="15" t="s">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="U35" s="15"/>
       <c r="V35" s="15"/>
@@ -5459,11 +5632,11 @@
       <c r="AM35" s="15"/>
       <c r="AN35" s="15"/>
       <c r="AO35" s="15" t="s">
-        <v>318</v>
+        <v>294</v>
       </c>
       <c r="AP35" s="15"/>
       <c r="AQ35" s="15" t="s">
-        <v>299</v>
+        <v>275</v>
       </c>
       <c r="AR35" s="15"/>
       <c r="AS35" s="15"/>
@@ -5477,19 +5650,19 @@
       <c r="BA35" s="15"/>
       <c r="BB35" s="15"/>
       <c r="BC35" s="15" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="BD35" s="15" t="s">
         <v>118</v>
       </c>
       <c r="BE35" s="15" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
       <c r="BF35" s="15" t="s">
         <v>119</v>
       </c>
       <c r="BG35" s="15" t="s">
-        <v>384</v>
+        <v>360</v>
       </c>
       <c r="BH35" s="15"/>
       <c r="BI35" s="15"/>
@@ -5607,18 +5780,18 @@
       </c>
       <c r="N37" s="15"/>
       <c r="O37" s="15" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="P37" s="15"/>
       <c r="Q37" s="15"/>
       <c r="R37" s="15" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="S37" s="15" t="s">
-        <v>275</v>
+        <v>251</v>
       </c>
       <c r="T37" s="15" t="s">
-        <v>276</v>
+        <v>252</v>
       </c>
       <c r="U37" s="15"/>
       <c r="V37" s="15"/>
@@ -5643,11 +5816,11 @@
       <c r="AM37" s="15"/>
       <c r="AN37" s="15"/>
       <c r="AO37" s="15" t="s">
-        <v>310</v>
+        <v>286</v>
       </c>
       <c r="AP37" s="15"/>
       <c r="AQ37" s="15" t="s">
-        <v>305</v>
+        <v>281</v>
       </c>
       <c r="AR37" s="15"/>
       <c r="AS37" s="15"/>
@@ -5661,13 +5834,13 @@
       <c r="BA37" s="15"/>
       <c r="BB37" s="15"/>
       <c r="BC37" s="15" t="s">
-        <v>329</v>
+        <v>305</v>
       </c>
       <c r="BD37" s="15" t="s">
         <v>122</v>
       </c>
       <c r="BE37" s="15" t="s">
-        <v>385</v>
+        <v>361</v>
       </c>
       <c r="BF37" s="15"/>
       <c r="BG37" s="15"/>
@@ -5779,18 +5952,18 @@
       </c>
       <c r="N39" s="15"/>
       <c r="O39" s="15" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="P39" s="15"/>
       <c r="Q39" s="15"/>
       <c r="R39" s="15" t="s">
-        <v>277</v>
+        <v>253</v>
       </c>
       <c r="S39" s="15" t="s">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="T39" s="15" t="s">
-        <v>278</v>
+        <v>254</v>
       </c>
       <c r="U39" s="15"/>
       <c r="V39" s="15"/>
@@ -5815,7 +5988,7 @@
       <c r="AM39" s="15"/>
       <c r="AN39" s="15"/>
       <c r="AO39" s="15" t="s">
-        <v>309</v>
+        <v>285</v>
       </c>
       <c r="AP39" s="15" t="s">
         <v>0</v>
@@ -5827,7 +6000,7 @@
         <v>0</v>
       </c>
       <c r="AS39" s="15" t="s">
-        <v>308</v>
+        <v>284</v>
       </c>
       <c r="AT39" s="15"/>
       <c r="AU39" s="15"/>
@@ -5961,18 +6134,18 @@
       </c>
       <c r="N41" s="15"/>
       <c r="O41" s="15" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="P41" s="15"/>
       <c r="Q41" s="15"/>
       <c r="R41" s="15" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="S41" s="15" t="s">
         <v>0</v>
       </c>
       <c r="T41" s="15" t="s">
-        <v>280</v>
+        <v>256</v>
       </c>
       <c r="U41" s="15"/>
       <c r="V41" s="15"/>
@@ -5997,11 +6170,11 @@
       <c r="AM41" s="15"/>
       <c r="AN41" s="15"/>
       <c r="AO41" s="15" t="s">
-        <v>310</v>
+        <v>286</v>
       </c>
       <c r="AP41" s="15"/>
       <c r="AQ41" s="15" t="s">
-        <v>305</v>
+        <v>281</v>
       </c>
       <c r="AR41" s="15"/>
       <c r="AS41" s="15" t="s">
@@ -6129,7 +6302,7 @@
       <c r="K43" s="15"/>
       <c r="L43" s="15"/>
       <c r="M43" s="15" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="N43" s="15" t="s">
         <v>0</v>
@@ -6156,7 +6329,7 @@
         <v>0</v>
       </c>
       <c r="V43" s="15" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="W43" s="15"/>
       <c r="X43" s="15"/>
@@ -6181,13 +6354,13 @@
       <c r="AO43" s="15"/>
       <c r="AP43" s="15"/>
       <c r="AQ43" s="15" t="s">
-        <v>306</v>
+        <v>282</v>
       </c>
       <c r="AR43" s="15" t="s">
         <v>0</v>
       </c>
       <c r="AS43" s="15" t="s">
-        <v>307</v>
+        <v>283</v>
       </c>
       <c r="AT43" s="15"/>
       <c r="AU43" s="15"/>
@@ -6199,7 +6372,7 @@
       <c r="BA43" s="15"/>
       <c r="BB43" s="15"/>
       <c r="BC43" s="15" t="s">
-        <v>332</v>
+        <v>308</v>
       </c>
       <c r="BD43" s="15"/>
       <c r="BE43" s="15"/>
@@ -6397,7 +6570,7 @@
       <c r="T46" s="15"/>
       <c r="U46" s="15"/>
       <c r="V46" s="15" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="W46" s="15" t="s">
         <v>0</v>
@@ -6415,7 +6588,7 @@
         <v>0</v>
       </c>
       <c r="AB46" s="15" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="AC46" s="15"/>
       <c r="AD46" s="15"/>
@@ -6520,7 +6693,7 @@
       <c r="BA47" s="15"/>
       <c r="BB47" s="15"/>
       <c r="BC47" s="15" t="s">
-        <v>334</v>
+        <v>310</v>
       </c>
       <c r="BD47" s="15" t="s">
         <v>136</v>
@@ -6713,37 +6886,38 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="beginsWith" dxfId="6" priority="1" operator="beginsWith" text="FO">
+    <cfRule type="beginsWith" dxfId="15" priority="2" operator="beginsWith" text="FO">
       <formula>LEFT(A1,LEN("FO"))="FO"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="5" priority="2" operator="beginsWith" text="|">
+    <cfRule type="beginsWith" dxfId="14" priority="3" operator="beginsWith" text="|">
       <formula>LEFT(A1,LEN("|"))="|"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="5" operator="beginsWith" text="OT">
+    <cfRule type="beginsWith" dxfId="13" priority="6" operator="beginsWith" text="OT">
       <formula>LEFT(A1,LEN("OT"))="OT"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="6" operator="beginsWith" text="HQ">
+    <cfRule type="beginsWith" dxfId="12" priority="7" operator="beginsWith" text="HQ">
       <formula>LEFT(A1,LEN("HQ"))="HQ"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="2" priority="9">
+    <cfRule type="containsBlanks" dxfId="11" priority="10">
       <formula>LEN(TRIM(A1))=0</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="8" priority="1" operator="beginsWith" text="PL">
+      <formula>LEFT(A1,LEN("PL"))="PL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="beginsWith" dxfId="1" priority="4" operator="beginsWith" text="CT">
+    <cfRule type="beginsWith" dxfId="10" priority="5" operator="beginsWith" text="CT">
       <formula>LEFT(A1,LEN("CT"))="CT"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="beginsWith" dxfId="0" priority="3" operator="beginsWith" text="AP">
+    <cfRule type="beginsWith" dxfId="9" priority="4" operator="beginsWith" text="AP">
       <formula>LEFT(A1,LEN("AP"))="AP"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -6754,11 +6928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E986"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-    <sheetView topLeftCell="A24" workbookViewId="1">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0"/>
@@ -6777,10 +6948,10 @@
         <v>HQ1</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>446</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="48" customHeight="1">
@@ -6789,10 +6960,10 @@
         <v>HQ2</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>152</v>
+        <v>447</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D2" s="25"/>
     </row>
@@ -6802,10 +6973,10 @@
         <v>HQ3</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>154</v>
+        <v>448</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="96" customHeight="1">
@@ -6814,16 +6985,16 @@
         <v>HQ4</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>156</v>
+        <v>449</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>467</v>
+        <v>443</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>466</v>
+        <v>442</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="96" customHeight="1">
@@ -6832,10 +7003,10 @@
         <v>HQ5</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>158</v>
+        <v>450</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D5" s="25"/>
     </row>
@@ -6845,10 +7016,10 @@
         <v>HQ6</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>160</v>
+        <v>451</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D6" s="25"/>
     </row>
@@ -6858,7 +7029,7 @@
         <v>HQ7</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>162</v>
+        <v>452</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="25"/>
@@ -6869,16 +7040,16 @@
         <v>HQ8</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>163</v>
+        <v>453</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>468</v>
+        <v>444</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>465</v>
+        <v>441</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="48" customHeight="1">
@@ -6887,11 +7058,11 @@
         <v>HQ9</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>165</v>
+        <v>454</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="25" t="s">
-        <v>469</v>
+        <v>445</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="48" customHeight="1">
@@ -6906,7 +7077,7 @@
         <v>BK1</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>171</v>
+        <v>455</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="26"/>
@@ -6917,7 +7088,7 @@
         <v>BK2</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>167</v>
+        <v>456</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="25"/>
@@ -6928,7 +7099,7 @@
         <v>BK3</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>168</v>
+        <v>456</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="25"/>
@@ -6939,7 +7110,7 @@
         <v>BK4</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>169</v>
+        <v>456</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="25"/>
@@ -6950,7 +7121,7 @@
         <v>BK5</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>170</v>
+        <v>456</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="27"/>
@@ -6961,7 +7132,7 @@
         <v>BK6</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>166</v>
+        <v>456</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="25"/>
@@ -6984,7 +7155,7 @@
         <v>OT1</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>172</v>
+        <v>457</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="27"/>
@@ -6995,7 +7166,7 @@
         <v>OT2</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>173</v>
+        <v>458</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="25"/>
@@ -7006,7 +7177,7 @@
         <v>OT3</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>174</v>
+        <v>459</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="25"/>
@@ -7017,10 +7188,10 @@
         <v>OT4</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>179</v>
+        <v>460</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>447</v>
+        <v>423</v>
       </c>
       <c r="D22" s="25"/>
     </row>
@@ -7030,10 +7201,10 @@
         <v>OT5</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>179</v>
+        <v>460</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>447</v>
+        <v>423</v>
       </c>
       <c r="D23" s="25"/>
     </row>
@@ -7043,7 +7214,7 @@
         <v>OT6</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>174</v>
+        <v>459</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="25"/>
@@ -7054,7 +7225,7 @@
         <v>OT7</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>176</v>
+        <v>461</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="25"/>
@@ -7065,7 +7236,7 @@
         <v>OT8</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>175</v>
+        <v>461</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="25"/>
@@ -7076,7 +7247,7 @@
         <v>OT9</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>177</v>
+        <v>462</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="25"/>
@@ -7087,7 +7258,7 @@
         <v>OT10</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>175</v>
+        <v>461</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="48" customHeight="1">
@@ -7096,7 +7267,7 @@
         <v>OT11</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>178</v>
+        <v>462</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="48" customHeight="1">
@@ -7105,7 +7276,7 @@
         <v>OT12</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>177</v>
+        <v>462</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="48" customHeight="1">
@@ -7114,7 +7285,7 @@
         <v>OT13</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>177</v>
+        <v>462</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="48" customHeight="1">
@@ -7123,7 +7294,7 @@
         <v>OT14</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>180</v>
+        <v>462</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="48" customHeight="1">
@@ -10843,7 +11014,6 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -10857,9 +11027,6 @@
     <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
-    <sheetView topLeftCell="A34" workbookViewId="1">
-      <selection activeCell="B24" sqref="B24"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="47" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -10871,13 +11038,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="48" customHeight="1">
       <c r="A1" s="10" t="s">
-        <v>281</v>
+        <v>257</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>396</v>
+        <v>372</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="47" customHeight="1">
@@ -10886,10 +11053,10 @@
         <v>CT2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>396</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="47" customHeight="1">
@@ -10898,10 +11065,10 @@
         <v>CT3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>397</v>
+        <v>373</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="47" customHeight="1">
@@ -10910,10 +11077,10 @@
         <v>CT4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="47" customHeight="1">
@@ -10922,10 +11089,10 @@
         <v>CT5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="47" customHeight="1">
@@ -10934,10 +11101,10 @@
         <v>CT6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="47" customHeight="1">
@@ -10946,10 +11113,10 @@
         <v>CT7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>399</v>
+        <v>375</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="47" customHeight="1">
@@ -10958,10 +11125,10 @@
         <v>CT8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="47" customHeight="1">
@@ -10970,10 +11137,10 @@
         <v>CT9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="47" customHeight="1">
@@ -10982,10 +11149,10 @@
         <v>CT10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="47" customHeight="1">
@@ -10994,10 +11161,10 @@
         <v>CT11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="47" customHeight="1">
@@ -11006,10 +11173,10 @@
         <v>CT12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="47" customHeight="1">
@@ -11018,10 +11185,10 @@
         <v>CT13</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>400</v>
+        <v>376</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="47" customHeight="1">
@@ -11030,10 +11197,10 @@
         <v>CT14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="47" customHeight="1">
@@ -11042,10 +11209,10 @@
         <v>CT15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="47" customHeight="1">
@@ -11054,10 +11221,10 @@
         <v>CT16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>394</v>
+        <v>370</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>395</v>
+        <v>371</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="47" customHeight="1">
@@ -11072,13 +11239,13 @@
     </row>
     <row r="19" spans="1:3" ht="96" customHeight="1">
       <c r="A19" s="14" t="s">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="47" customHeight="1">
@@ -11087,10 +11254,10 @@
         <v>AP2</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="47" customHeight="1">
@@ -11099,10 +11266,10 @@
         <v>AP3</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="47" customHeight="1">
@@ -11111,10 +11278,10 @@
         <v>AP4</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="47" customHeight="1">
@@ -11123,10 +11290,10 @@
         <v>AP5</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="47" customHeight="1">
@@ -11135,10 +11302,10 @@
         <v>AP6</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="47" customHeight="1">
@@ -11147,10 +11314,10 @@
         <v>AP7</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="47" customHeight="1">
@@ -11159,10 +11326,10 @@
         <v>AP8</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>239</v>
+        <v>215</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="47" customHeight="1">
@@ -11171,10 +11338,10 @@
         <v>AP9</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="47" customHeight="1">
@@ -11183,10 +11350,10 @@
         <v>AP10</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="47" customHeight="1">
@@ -11195,10 +11362,10 @@
         <v>AP11</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>245</v>
+        <v>221</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="47" customHeight="1">
@@ -11207,10 +11374,10 @@
         <v>AP12</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="47" customHeight="1">
@@ -11219,10 +11386,10 @@
         <v>AP13</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="47" customHeight="1">
@@ -11231,10 +11398,10 @@
         <v>AP14</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="47" customHeight="1">
@@ -11243,10 +11410,10 @@
         <v>AP15</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="47" customHeight="1">
@@ -11255,10 +11422,10 @@
         <v>AP16</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="47" customHeight="1">
@@ -11267,10 +11434,10 @@
         <v>AP17</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="47" customHeight="1">
@@ -11285,215 +11452,215 @@
     </row>
     <row r="38" spans="1:3" ht="47" customHeight="1">
       <c r="A38" s="14" t="s">
-        <v>404</v>
+        <v>380</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>427</v>
+        <v>403</v>
       </c>
       <c r="C38" s="5"/>
     </row>
     <row r="39" spans="1:3" ht="47" customHeight="1">
       <c r="A39" s="14" t="s">
-        <v>405</v>
+        <v>381</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="5"/>
     </row>
     <row r="40" spans="1:3" ht="47" customHeight="1">
       <c r="A40" s="14" t="s">
-        <v>406</v>
+        <v>382</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>431</v>
+        <v>407</v>
       </c>
       <c r="C40" s="5"/>
     </row>
     <row r="41" spans="1:3" ht="47" customHeight="1">
       <c r="A41" s="14" t="s">
-        <v>407</v>
+        <v>383</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>432</v>
+        <v>408</v>
       </c>
       <c r="C41" s="5"/>
     </row>
     <row r="42" spans="1:3" ht="47" customHeight="1">
       <c r="A42" s="14" t="s">
-        <v>408</v>
+        <v>384</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>428</v>
+        <v>404</v>
       </c>
       <c r="C42" s="5"/>
     </row>
     <row r="43" spans="1:3" ht="47" customHeight="1">
       <c r="A43" s="14" t="s">
-        <v>409</v>
+        <v>385</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>429</v>
+        <v>405</v>
       </c>
       <c r="C43" s="5"/>
     </row>
     <row r="44" spans="1:3" ht="47" customHeight="1">
       <c r="A44" s="14" t="s">
-        <v>410</v>
+        <v>386</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>430</v>
+        <v>406</v>
       </c>
       <c r="C44" s="5"/>
     </row>
     <row r="45" spans="1:3" ht="47" customHeight="1">
       <c r="A45" s="14" t="s">
-        <v>411</v>
+        <v>387</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="C45" s="5"/>
     </row>
     <row r="46" spans="1:3" ht="47" customHeight="1">
       <c r="A46" s="14" t="s">
-        <v>412</v>
+        <v>388</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
       <c r="C46" s="5"/>
     </row>
     <row r="47" spans="1:3" ht="47" customHeight="1">
       <c r="A47" s="14" t="s">
-        <v>414</v>
+        <v>390</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>434</v>
+        <v>410</v>
       </c>
       <c r="C47" s="5"/>
     </row>
     <row r="48" spans="1:3" ht="47" customHeight="1">
       <c r="A48" s="14" t="s">
-        <v>415</v>
+        <v>391</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>435</v>
+        <v>411</v>
       </c>
       <c r="C48" s="5"/>
     </row>
     <row r="49" spans="1:3" ht="47" customHeight="1">
       <c r="A49" s="14" t="s">
-        <v>416</v>
+        <v>392</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>436</v>
+        <v>412</v>
       </c>
       <c r="C49" s="5"/>
     </row>
     <row r="50" spans="1:3" ht="47" customHeight="1">
       <c r="A50" s="14" t="s">
-        <v>417</v>
+        <v>393</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>434</v>
+        <v>410</v>
       </c>
       <c r="C50" s="5"/>
     </row>
     <row r="51" spans="1:3" ht="47" customHeight="1">
       <c r="A51" s="14" t="s">
-        <v>418</v>
+        <v>394</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>437</v>
+        <v>413</v>
       </c>
       <c r="C51" s="5"/>
     </row>
     <row r="52" spans="1:3" ht="47" customHeight="1">
       <c r="A52" s="14" t="s">
-        <v>433</v>
+        <v>409</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>438</v>
+        <v>414</v>
       </c>
       <c r="C52" s="5"/>
     </row>
     <row r="53" spans="1:3" ht="47" customHeight="1">
       <c r="A53" s="14" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="C53" s="5"/>
     </row>
     <row r="54" spans="1:3" ht="47" customHeight="1">
       <c r="A54" s="14" t="s">
-        <v>420</v>
+        <v>396</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>439</v>
+        <v>415</v>
       </c>
       <c r="C54" s="5"/>
     </row>
     <row r="55" spans="1:3" ht="47" customHeight="1">
       <c r="A55" s="14" t="s">
-        <v>421</v>
+        <v>397</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>440</v>
+        <v>416</v>
       </c>
       <c r="C55" s="5"/>
     </row>
     <row r="56" spans="1:3" ht="47" customHeight="1">
       <c r="A56" s="14" t="s">
-        <v>422</v>
+        <v>398</v>
       </c>
       <c r="B56" s="21" t="s">
-        <v>441</v>
+        <v>417</v>
       </c>
       <c r="C56" s="5"/>
     </row>
     <row r="57" spans="1:3" ht="47" customHeight="1">
       <c r="A57" s="14" t="s">
-        <v>423</v>
+        <v>399</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>439</v>
+        <v>415</v>
       </c>
       <c r="C57" s="5"/>
     </row>
     <row r="58" spans="1:3" ht="47" customHeight="1">
       <c r="A58" s="14" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>442</v>
+        <v>418</v>
       </c>
       <c r="C58" s="5"/>
     </row>
     <row r="59" spans="1:3" ht="47" customHeight="1">
       <c r="A59" s="14" t="s">
-        <v>425</v>
+        <v>401</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>443</v>
+        <v>419</v>
       </c>
       <c r="C59" s="5"/>
     </row>
     <row r="60" spans="1:3" ht="47" customHeight="1">
       <c r="A60" s="14" t="s">
-        <v>419</v>
+        <v>395</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>444</v>
+        <v>420</v>
       </c>
       <c r="C60" s="5"/>
     </row>
     <row r="61" spans="1:3" ht="47" customHeight="1">
       <c r="A61" s="14" t="s">
-        <v>426</v>
+        <v>402</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>445</v>
+        <v>421</v>
       </c>
       <c r="C61" s="5"/>
     </row>
@@ -11519,13 +11686,13 @@
     </row>
     <row r="66" spans="1:3" ht="47" customHeight="1">
       <c r="A66" s="14" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>446</v>
+        <v>422</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="47" customHeight="1">
@@ -11534,10 +11701,10 @@
         <v>SW2</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>446</v>
+        <v>422</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="47" customHeight="1">
@@ -11546,10 +11713,10 @@
         <v>SW3</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>446</v>
+        <v>422</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>261</v>
+        <v>237</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="47" customHeight="1">
@@ -11558,10 +11725,10 @@
         <v>SW4</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>446</v>
+        <v>422</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>262</v>
+        <v>238</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="47" customHeight="1">
@@ -15424,7 +15591,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -15438,9 +15604,6 @@
     <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="1">
-      <selection activeCell="B27" sqref="B27"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -15452,626 +15615,626 @@
   <sheetData>
     <row r="1" spans="1:2" ht="48" customHeight="1">
       <c r="A1" s="8" t="s">
-        <v>324</v>
+        <v>300</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="48" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="48" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>326</v>
+        <v>302</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="48" customHeight="1">
       <c r="A4" s="8" t="s">
-        <v>327</v>
+        <v>303</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="48" customHeight="1">
       <c r="A5" s="8" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="48" customHeight="1">
       <c r="A6" s="8" t="s">
-        <v>329</v>
+        <v>305</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="48" customHeight="1">
       <c r="A7" s="8" t="s">
-        <v>330</v>
+        <v>306</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="48" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="48" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>332</v>
+        <v>308</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="48" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="48" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>334</v>
+        <v>310</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="48" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>335</v>
+        <v>311</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="48" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="48" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>337</v>
+        <v>313</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="48" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="48" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>339</v>
+        <v>315</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="48" customHeight="1">
       <c r="A17" s="8" t="s">
-        <v>340</v>
+        <v>316</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="48" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="48" customHeight="1">
       <c r="A19" s="8" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="48" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="48" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>344</v>
+        <v>320</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="48" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="48" customHeight="1">
       <c r="A23" s="8" t="s">
-        <v>346</v>
+        <v>322</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="48" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="48" customHeight="1">
       <c r="A25" s="8" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="48" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="48" customHeight="1">
       <c r="A29" s="8" t="s">
-        <v>448</v>
+        <v>424</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>452</v>
+        <v>428</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="48" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>449</v>
+        <v>425</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>452</v>
+        <v>428</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="48" customHeight="1">
       <c r="A31" s="8" t="s">
-        <v>381</v>
+        <v>357</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>452</v>
+        <v>428</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="48" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>379</v>
+        <v>355</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>452</v>
+        <v>428</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="48" customHeight="1">
       <c r="A33" s="8" t="s">
-        <v>450</v>
+        <v>426</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>452</v>
+        <v>428</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="48" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>378</v>
+        <v>354</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>452</v>
+        <v>428</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="48" customHeight="1">
       <c r="A35" s="8" t="s">
-        <v>377</v>
+        <v>353</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>452</v>
+        <v>428</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="48" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>380</v>
+        <v>356</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>452</v>
+        <v>428</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="48" customHeight="1">
       <c r="A37" s="8" t="s">
-        <v>382</v>
+        <v>358</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>452</v>
+        <v>428</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="48" customHeight="1">
       <c r="A38" s="8" t="s">
-        <v>451</v>
+        <v>427</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>452</v>
+        <v>428</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="48" customHeight="1">
       <c r="A39" s="8" t="s">
-        <v>384</v>
+        <v>360</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>452</v>
+        <v>428</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="48" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>452</v>
+        <v>428</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="48" customHeight="1">
       <c r="A41" s="8" t="s">
-        <v>385</v>
+        <v>361</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>452</v>
+        <v>428</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="48" customHeight="1">
       <c r="A45" s="8" t="s">
-        <v>390</v>
+        <v>366</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>453</v>
+        <v>429</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="48" customHeight="1">
       <c r="A46" s="8" t="s">
-        <v>386</v>
+        <v>362</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>454</v>
+        <v>430</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="48" customHeight="1">
       <c r="A47" s="8" t="s">
-        <v>391</v>
+        <v>367</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>455</v>
+        <v>431</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="48" customHeight="1">
       <c r="A48" s="8" t="s">
-        <v>387</v>
+        <v>363</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>456</v>
+        <v>432</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="48" customHeight="1">
       <c r="A49" s="8" t="s">
-        <v>388</v>
+        <v>364</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>457</v>
+        <v>433</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="48" customHeight="1">
       <c r="A50" s="8" t="s">
-        <v>389</v>
+        <v>365</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>458</v>
+        <v>434</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="48" customHeight="1">
       <c r="A51" s="8" t="s">
-        <v>392</v>
+        <v>368</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>458</v>
+        <v>434</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="48" customHeight="1">
       <c r="A54" s="8" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="48" customHeight="1">
       <c r="A55" s="8" t="s">
-        <v>354</v>
+        <v>330</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="48" customHeight="1">
       <c r="A56" s="8" t="s">
-        <v>363</v>
+        <v>339</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="48" customHeight="1">
       <c r="A57" s="8" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="48" customHeight="1">
       <c r="A58" s="8" t="s">
-        <v>353</v>
+        <v>329</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="48" customHeight="1">
       <c r="A59" s="8" t="s">
-        <v>352</v>
+        <v>328</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="48" customHeight="1">
       <c r="A60" s="8" t="s">
-        <v>356</v>
+        <v>332</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="48" customHeight="1">
       <c r="A61" s="8" t="s">
-        <v>355</v>
+        <v>331</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="48" customHeight="1">
       <c r="A62" s="8" t="s">
-        <v>361</v>
+        <v>337</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="48" customHeight="1">
       <c r="A63" s="8" t="s">
-        <v>362</v>
+        <v>338</v>
       </c>
       <c r="B63" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="48" customHeight="1">
       <c r="A64" s="8" t="s">
-        <v>360</v>
+        <v>336</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="48" customHeight="1">
       <c r="A65" s="8" t="s">
-        <v>351</v>
+        <v>327</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="48" customHeight="1">
       <c r="A66" s="8" t="s">
-        <v>350</v>
+        <v>326</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="48" customHeight="1">
       <c r="A67" s="8" t="s">
-        <v>459</v>
+        <v>435</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="48" customHeight="1">
       <c r="A68" s="8" t="s">
-        <v>359</v>
+        <v>335</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="48" customHeight="1">
       <c r="A69" s="8" t="s">
-        <v>460</v>
+        <v>436</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="48" customHeight="1">
       <c r="A70" s="8" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="48" customHeight="1">
       <c r="A71" s="8" t="s">
-        <v>367</v>
+        <v>343</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="48" customHeight="1">
       <c r="A72" s="8" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="48" customHeight="1">
       <c r="A73" s="8" t="s">
-        <v>372</v>
+        <v>348</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="48" customHeight="1">
       <c r="A74" s="8" t="s">
-        <v>368</v>
+        <v>344</v>
       </c>
       <c r="B74" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="48" customHeight="1">
       <c r="A75" s="8" t="s">
-        <v>365</v>
+        <v>341</v>
       </c>
       <c r="B75" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="48" customHeight="1">
       <c r="A76" s="8" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="B76" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="48" customHeight="1">
       <c r="A77" s="8" t="s">
-        <v>369</v>
+        <v>345</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="48" customHeight="1">
       <c r="A78" s="8" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
       <c r="B78" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="48" customHeight="1">
       <c r="A79" s="8" t="s">
-        <v>461</v>
+        <v>437</v>
       </c>
       <c r="B79" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="48" customHeight="1">
       <c r="A80" s="8" t="s">
-        <v>370</v>
+        <v>346</v>
       </c>
       <c r="B80" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="48" customHeight="1">
       <c r="A81" s="8" t="s">
-        <v>375</v>
+        <v>351</v>
       </c>
       <c r="B81" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="48" customHeight="1">
       <c r="A82" s="8" t="s">
-        <v>462</v>
+        <v>438</v>
       </c>
       <c r="B82" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="48" customHeight="1">
       <c r="A83" s="8" t="s">
-        <v>463</v>
+        <v>439</v>
       </c>
       <c r="B83" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="48" customHeight="1">
       <c r="A84" s="8" t="s">
-        <v>376</v>
+        <v>352</v>
       </c>
       <c r="B84" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="48" customHeight="1">
       <c r="A85" s="8" t="s">
-        <v>374</v>
+        <v>350</v>
       </c>
       <c r="B85" s="19" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
   </sheetData>
@@ -16079,7 +16242,6 @@
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>